<commit_message>
fixed rounding bug that was making 1 not equal 1
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768E5618-49E7-0141-86EB-AC03B385A85D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E546DC84-7C47-A84B-B61B-ACFA029E8E97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20480" yWindow="460" windowWidth="20480" windowHeight="22580" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" activeTab="1" xr2:uid="{4280EF40-83DF-704D-92F9-FBB332F203D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -1154,9 +1153,8 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1535,7 +1533,7 @@
         <v>135</v>
       </c>
       <c r="D23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="s">
         <v>158</v>
@@ -1653,9 +1651,6 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="1">
-      <selection activeCell="G36" sqref="G36:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3512,7 +3507,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5:E73"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
updated results for docs 18 November
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0F8618-935D-1E47-8C3D-1BE59FE5262C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC892D9-8451-F540-B69C-8FE92DDF90A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20480" yWindow="460" windowWidth="20480" windowHeight="22580" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Self-report'!$E$1:$E$67</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="328">
   <si>
     <t>NumberFrom</t>
   </si>
@@ -821,9 +821,6 @@
     <t xml:space="preserve">Georgia FIND </t>
   </si>
   <si>
-    <t>WHO CHOICE in 2010</t>
-  </si>
-  <si>
     <t>Leave out for now</t>
   </si>
   <si>
@@ -836,15 +833,6 @@
     <t>LIFER study - removed pre treatment stuff from 338 total</t>
   </si>
   <si>
-    <t>(m-m*n)[*a*c]</t>
-  </si>
-  <si>
-    <t>(1-m-o)[*a*c]</t>
-  </si>
-  <si>
-    <t>(m*n+o)[*a*c]</t>
-  </si>
-  <si>
     <t>(1-w)*z3</t>
   </si>
   <si>
@@ -884,9 +872,6 @@
     <t>Nyasha's paper</t>
   </si>
   <si>
-    <t>WHO CHOICE in 2010 (also have other options from Nyasha's paper)</t>
-  </si>
-  <si>
     <t>Cost of distributing self test</t>
   </si>
   <si>
@@ -935,9 +920,6 @@
     <t>Liu 2019 systematic review</t>
   </si>
   <si>
-    <t>WHO choice</t>
-  </si>
-  <si>
     <t>4633 tests returned out of 4781 delivered</t>
   </si>
   <si>
@@ -1010,9 +992,6 @@
     <t>Seems high - but what about per year?</t>
   </si>
   <si>
-    <t>WHO Choice - but don't need?</t>
-  </si>
-  <si>
     <t>RDS cost data - test only</t>
   </si>
   <si>
@@ -1020,6 +999,30 @@
   </si>
   <si>
     <t>Guess for now, to update from DRIVE C questionnaire 8.1</t>
+  </si>
+  <si>
+    <t>(m-m*o)[*a*c]</t>
+  </si>
+  <si>
+    <t>(1-m-n)[*a*c]</t>
+  </si>
+  <si>
+    <t>(n+m*o)[*a*c]</t>
+  </si>
+  <si>
+    <t>WHO CHOICE in 2010 is 7.82</t>
+  </si>
+  <si>
+    <t>WHO CHOICE in 2010 is 2.91 (also have other options from Nyasha's paper)</t>
+  </si>
+  <si>
+    <t>WHO choice is 10.74</t>
+  </si>
+  <si>
+    <t>WHO Choice - but don't need? 5.09</t>
+  </si>
+  <si>
+    <t>The Due 2020</t>
   </si>
 </sst>
 </file>
@@ -1400,20 +1403,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707EB61A-F669-6B48-8A71-B654C41C6040}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="89" hidden="1" customWidth="1"/>
+    <col min="7" max="12" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -1427,7 +1427,7 @@
         <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E1" t="s">
         <v>238</v>
@@ -1436,22 +1436,22 @@
         <v>239</v>
       </c>
       <c r="G1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="I1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="J1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="K1" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="L1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="M1" t="s">
         <v>106</v>
@@ -1482,19 +1482,19 @@
         <v>13450</v>
       </c>
       <c r="H2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I2">
         <v>17000</v>
       </c>
       <c r="J2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="K2">
         <v>5000</v>
       </c>
       <c r="L2" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="M2" t="s">
         <v>176</v>
@@ -1523,19 +1523,19 @@
         <v>0.109</v>
       </c>
       <c r="H3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="I3">
         <v>6.7000000000000002E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="K3" s="1">
         <v>0.6</v>
       </c>
       <c r="L3" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1561,19 +1561,19 @@
         <v>0.71</v>
       </c>
       <c r="H4" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I4" s="1">
         <v>0.8</v>
       </c>
       <c r="J4" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="K4" s="1">
         <v>0.7</v>
       </c>
       <c r="L4" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1599,7 +1599,7 @@
         <v>0.77400000000000002</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I5" s="1">
         <v>0.75</v>
@@ -1609,7 +1609,7 @@
         <v>0.84</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="M5" t="s">
         <v>142</v>
@@ -1638,7 +1638,7 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -1670,22 +1670,22 @@
         <v>14.55</v>
       </c>
       <c r="H7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I7">
         <v>36.590000000000003</v>
       </c>
       <c r="J7" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="K7" s="5">
         <v>2.2200000000000002</v>
       </c>
       <c r="L7" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="M7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1711,7 +1711,7 @@
         <v>78.5</v>
       </c>
       <c r="H8" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I8">
         <v>50</v>
@@ -1723,7 +1723,7 @@
         <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1743,25 +1743,28 @@
         <v>285</v>
       </c>
       <c r="F9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G9">
         <v>1552</v>
       </c>
       <c r="H9" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I9">
         <v>8000</v>
       </c>
       <c r="J9" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="K9">
         <v>122</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>160</v>
       </c>
@@ -1775,28 +1778,28 @@
         <v>5</v>
       </c>
       <c r="E10">
-        <v>7.82</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>260</v>
+        <v>323</v>
       </c>
       <c r="G10">
-        <v>2.91</v>
+        <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>281</v>
+        <v>324</v>
       </c>
       <c r="I10">
-        <v>10.74</v>
+        <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>298</v>
+        <v>325</v>
       </c>
       <c r="K10">
-        <v>5.09</v>
+        <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1816,13 +1819,13 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1877,13 +1880,13 @@
         <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G13">
         <v>59</v>
       </c>
       <c r="H13" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1916,19 +1919,19 @@
         <v>0.5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="I14" s="1">
         <v>0.1</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="K14" s="1">
         <v>0.5</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="M14" t="s">
         <v>145</v>
@@ -1994,7 +1997,7 @@
         <v>0.05</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="I16" s="1">
         <v>0.05</v>
@@ -2032,22 +2035,22 @@
         <v>0.99</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="I17" s="1">
         <v>0.9</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="K17" s="1">
         <v>1</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="M17" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -2081,7 +2084,7 @@
         <v>0.88700000000000001</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -2107,7 +2110,7 @@
         <v>0.92</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="I19" s="1">
         <v>0.9</v>
@@ -2117,10 +2120,10 @@
         <v>0.96</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="M19" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -2155,7 +2158,7 @@
         <v>0.92</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -2189,10 +2192,10 @@
         <v>0.05</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>170</v>
       </c>
@@ -2277,19 +2280,19 @@
         <v>0.9</v>
       </c>
       <c r="H24" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="I24" s="1">
         <v>0.96</v>
       </c>
       <c r="J24" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="K24" s="1">
         <v>0.46</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="M24" t="s">
         <v>146</v>
@@ -2318,19 +2321,19 @@
         <v>0.92</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="I25" s="1">
         <v>0.96</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="K25" s="1">
         <v>0.84</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="M25" t="s">
         <v>148</v>
@@ -2378,7 +2381,7 @@
         <v>175</v>
       </c>
       <c r="B27" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C27" t="s">
         <v>102</v>
@@ -2396,7 +2399,7 @@
         <v>14.12</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="I27" s="5">
         <v>0.18</v>
@@ -2406,7 +2409,7 @@
         <v>1</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -2430,14 +2433,14 @@
         <v>0.8</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="I28" s="1">
         <f>4633/4781</f>
         <v>0.96904413302656345</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="K28" s="1">
         <v>0.9</v>
@@ -2470,7 +2473,7 @@
         <v>0.96904413302656345</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="K29" s="1">
         <v>0.05</v>
@@ -2503,13 +2506,13 @@
         <v>0.96904413302656345</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="K30" s="1">
         <v>0.5</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -2521,8 +2524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D1F24D-5226-E34A-88F5-702AF231CD7B}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2584,7 +2587,7 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>265</v>
+        <v>320</v>
       </c>
       <c r="H2" s="1">
         <v>0.2</v>
@@ -2613,7 +2616,7 @@
         <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>266</v>
+        <v>321</v>
       </c>
       <c r="H3" s="1">
         <v>0.7</v>
@@ -2630,7 +2633,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -2642,7 +2645,7 @@
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>267</v>
+        <v>322</v>
       </c>
       <c r="H4" s="1">
         <v>0.1</v>
@@ -3035,7 +3038,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -3053,12 +3056,12 @@
         <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B20">
         <v>20</v>
@@ -3079,7 +3082,7 @@
         <v>256</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="I20" t="s">
         <v>180</v>
@@ -3087,7 +3090,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -3108,12 +3111,12 @@
         <v>255</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B22">
         <v>20</v>
@@ -3134,12 +3137,12 @@
         <v>253</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B23">
         <v>20</v>
@@ -3157,10 +3160,10 @@
         <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="I23" t="s">
         <v>116</v>
@@ -4338,6 +4341,7 @@
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updates for 7 December document
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FF4B75-2380-6E4A-AA86-970A4ED9254F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E104F5-7086-FB4C-B620-D34628CFB00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Peer-led" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parameters!$A$1:$M$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Self-report'!$E$1:$E$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="331">
   <si>
     <t>NumberFrom</t>
   </si>
@@ -929,9 +930,6 @@
     <t>Assume no difference</t>
   </si>
   <si>
-    <t>Jason's study but this includes all overheads</t>
-  </si>
-  <si>
     <t>FIND usability</t>
   </si>
   <si>
@@ -941,9 +939,6 @@
     <t>FIND usability - 4% needed assistance</t>
   </si>
   <si>
-    <t>drugs only from Chen 2018 (this is not very good)</t>
-  </si>
-  <si>
     <t>Ask Jason - previously tested?</t>
   </si>
   <si>
@@ -1026,6 +1021,18 @@
   </si>
   <si>
     <t>ytest</t>
+  </si>
+  <si>
+    <t>from Chen personal communication</t>
+  </si>
+  <si>
+    <t>based on Chen RDT</t>
+  </si>
+  <si>
+    <t>g.svr</t>
+  </si>
+  <si>
+    <t>PCRsvr</t>
   </si>
 </sst>
 </file>
@@ -1404,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707EB61A-F669-6B48-8A71-B654C41C6040}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1430,7 +1437,7 @@
         <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E1" t="s">
         <v>238</v>
@@ -1451,10 +1458,10 @@
         <v>290</v>
       </c>
       <c r="K1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M1" t="s">
         <v>106</v>
@@ -1497,7 +1504,7 @@
         <v>5000</v>
       </c>
       <c r="L2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="M2" t="s">
         <v>176</v>
@@ -1529,7 +1536,7 @@
         <v>274</v>
       </c>
       <c r="I3">
-        <v>6.7000000000000002E-3</v>
+        <v>0.01</v>
       </c>
       <c r="J3" t="s">
         <v>292</v>
@@ -1538,7 +1545,7 @@
         <v>0.6</v>
       </c>
       <c r="L3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1570,13 +1577,13 @@
         <v>0.8</v>
       </c>
       <c r="J4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K4" s="1">
         <v>0.7</v>
       </c>
       <c r="L4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1612,7 +1619,7 @@
         <v>0.84</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="M5" t="s">
         <v>142</v>
@@ -1632,22 +1639,22 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
         <v>244</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6" t="s">
         <v>275</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1676,16 +1683,16 @@
         <v>276</v>
       </c>
       <c r="I7">
-        <v>36.590000000000003</v>
+        <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>296</v>
+        <v>328</v>
       </c>
       <c r="K7" s="5">
         <v>2.2200000000000002</v>
       </c>
       <c r="L7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M7" t="s">
         <v>261</v>
@@ -1726,7 +1733,7 @@
         <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1755,16 +1762,16 @@
         <v>276</v>
       </c>
       <c r="I9">
-        <v>8000</v>
+        <v>2247</v>
       </c>
       <c r="J9" t="s">
-        <v>300</v>
+        <v>327</v>
       </c>
       <c r="K9">
         <v>122</v>
       </c>
       <c r="L9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1784,25 +1791,25 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
+        <v>321</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>322</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
         <v>323</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
         <v>324</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>325</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1928,13 +1935,13 @@
         <v>0.1</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K14" s="1">
         <v>0.5</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="M14" t="s">
         <v>145</v>
@@ -2044,13 +2051,13 @@
         <v>0.9</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K17" s="1">
         <v>1</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="M17" t="s">
         <v>284</v>
@@ -2087,7 +2094,7 @@
         <v>0.88700000000000001</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -2123,7 +2130,7 @@
         <v>0.96</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="M19" t="s">
         <v>284</v>
@@ -2161,7 +2168,7 @@
         <v>0.92</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -2195,7 +2202,7 @@
         <v>0.05</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -2289,13 +2296,13 @@
         <v>0.96</v>
       </c>
       <c r="J24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K24" s="1">
         <v>0.46</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="M24" t="s">
         <v>146</v>
@@ -2330,13 +2337,13 @@
         <v>0.96</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K25" s="1">
         <v>0.84</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="M25" t="s">
         <v>148</v>
@@ -2344,7 +2351,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B26" t="s">
         <v>181</v>
@@ -2412,7 +2419,7 @@
         <v>1</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -2515,7 +2522,33 @@
         <v>0.5</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>329</v>
+      </c>
+      <c r="B31" t="s">
+        <v>330</v>
+      </c>
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="E31">
+        <v>26.53</v>
+      </c>
+      <c r="G31">
+        <v>78.5</v>
+      </c>
+      <c r="I31">
+        <v>50</v>
+      </c>
+      <c r="K31">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2528,7 +2561,7 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2590,7 +2623,7 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H2" s="1">
         <v>0.2</v>
@@ -2619,7 +2652,7 @@
         <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H3" s="1">
         <v>0.7</v>
@@ -2648,7 +2681,7 @@
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H4" s="1">
         <v>0.1</v>

</xml_diff>

<commit_message>
updated results for version to send to Sonjelle and others
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E104F5-7086-FB4C-B620-D34628CFB00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FB2739-89C7-1F47-8AAF-D50E4BC0FA80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
-    <sheet name="Self-report" sheetId="2" r:id="rId2"/>
-    <sheet name="Peer-led" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Self-report" sheetId="2" r:id="rId3"/>
+    <sheet name="Peer-led" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parameters!$A$1:$M$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Self-report'!$E$1:$E$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parameters!$A$1:$Y$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Self-report'!$E$1:$E$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="354">
   <si>
     <t>NumberFrom</t>
   </si>
@@ -762,12 +763,6 @@
     <t>GeorgiaSource</t>
   </si>
   <si>
-    <t>Hagan 2019/Serosurvey</t>
-  </si>
-  <si>
-    <t>Google * Shaun (census 2014) - men 40-49</t>
-  </si>
-  <si>
     <t>Shaun 6.9/28.9</t>
   </si>
   <si>
@@ -804,9 +799,6 @@
     <t>(1-b)*w*z2</t>
   </si>
   <si>
-    <t>Placeholder as z1-z3 are used in next step</t>
-  </si>
-  <si>
     <t>b*(1-v)*w*z1</t>
   </si>
   <si>
@@ -819,9 +811,6 @@
     <t>i+j</t>
   </si>
   <si>
-    <t xml:space="preserve">Georgia FIND </t>
-  </si>
-  <si>
     <t>Leave out for now</t>
   </si>
   <si>
@@ -831,9 +820,6 @@
     <t>LIFER study (weighted average of diagnostic w FIB or elastography paid by government)</t>
   </si>
   <si>
-    <t>LIFER study - removed pre treatment stuff from 338 total</t>
-  </si>
-  <si>
     <t>(1-w)*z3</t>
   </si>
   <si>
@@ -861,12 +847,6 @@
     <t>KenyaSource</t>
   </si>
   <si>
-    <t>Jack's paper</t>
-  </si>
-  <si>
-    <t>Jack's paper (2015)/TLC</t>
-  </si>
-  <si>
     <t>Base case oral test</t>
   </si>
   <si>
@@ -882,9 +862,6 @@
     <t>Not account for this yet but do have some counselling within distribution cost</t>
   </si>
   <si>
-    <t>Mangenah 2019 - note it involves a demonstration of the test and counselling etc</t>
-  </si>
-  <si>
     <t>FIND usability (agreement with professional use test)</t>
   </si>
   <si>
@@ -918,9 +895,6 @@
     <t>Ong CE HIVST (not published yet?) - MSM population in Zhuhai</t>
   </si>
   <si>
-    <t>Liu 2019 systematic review</t>
-  </si>
-  <si>
     <t>4633 tests returned out of 4781 delivered</t>
   </si>
   <si>
@@ -954,12 +928,6 @@
     <t>VietnamSource</t>
   </si>
   <si>
-    <t>Des Jarlais 2018 - HaiPhong PWID</t>
-  </si>
-  <si>
-    <t>Moles 2020 (72% in DRIVE C)</t>
-  </si>
-  <si>
     <t>DRIVE C screening results</t>
   </si>
   <si>
@@ -978,9 +946,6 @@
     <t>FIND usability (but could be higher depending on distribution model)</t>
   </si>
   <si>
-    <t>Look at two scenarios one with help for testing</t>
-  </si>
-  <si>
     <t>Change for peer led model</t>
   </si>
   <si>
@@ -1017,22 +982,129 @@
     <t>WHO Choice - but don't need? 5.09</t>
   </si>
   <si>
-    <t>The Due 2020</t>
-  </si>
-  <si>
     <t>ytest</t>
   </si>
   <si>
-    <t>from Chen personal communication</t>
-  </si>
-  <si>
-    <t>based on Chen RDT</t>
-  </si>
-  <si>
     <t>g.svr</t>
   </si>
   <si>
     <t>PCRsvr</t>
+  </si>
+  <si>
+    <t>GeorgiaLow</t>
+  </si>
+  <si>
+    <t>GeorgiaHigh</t>
+  </si>
+  <si>
+    <t>Google * Shaun (census 2014) - men 40-49. Updated to 2020 estimates from Georgia Demographics.</t>
+  </si>
+  <si>
+    <t>Hagan 2019/Serosurvey - estimated boundaries from figure in Hagan 2019 - ask Shaun for update</t>
+  </si>
+  <si>
+    <t>Georgia FIND - 2018 USD (bounds are high and low estimates from different sites)</t>
+  </si>
+  <si>
+    <t>Georgia FIND - 2018 USD (they assume 10% SE)</t>
+  </si>
+  <si>
+    <t>CPI</t>
+  </si>
+  <si>
+    <t>2019 not available</t>
+  </si>
+  <si>
+    <t>LIFER study - removed pre treatment stuff from 338 total - 2017 USD</t>
+  </si>
+  <si>
+    <t>KenyaLow</t>
+  </si>
+  <si>
+    <t>KenyaHigh</t>
+  </si>
+  <si>
+    <t>Akiyama LancetID 2019 (10.9 was from Jack's unpublished)</t>
+  </si>
+  <si>
+    <t>Nyasha's paper - 2018 USD (SD bioline kit plus staff time for RDT visit)</t>
+  </si>
+  <si>
+    <t>Nyasha's paper - as above</t>
+  </si>
+  <si>
+    <t>Nyasha's paper - lowest cost considered. Take out pre treatment</t>
+  </si>
+  <si>
+    <t>Nyasha's paper - confirmatory result visit plus baseline initial assessment</t>
+  </si>
+  <si>
+    <t>ChinaLow</t>
+  </si>
+  <si>
+    <t>ChinaHigh</t>
+  </si>
+  <si>
+    <t>Assume approx $2 for postage and $1 for packaging ($1.60 estimated from Georgia post website for postage of a small package)</t>
+  </si>
+  <si>
+    <t>Mangenah 2019 - note it involves a demonstration of the test and counselling etc. 2017 USD. * 14% of total costs attributable to test cost itself in Zambia
+* Zambia has closest GDP per capita to Kenya
+* Base cost is $16.42 so $14.12 for everything but the test kit (discuss this assumption with Fern)</t>
+  </si>
+  <si>
+    <t>Liu 2019 systematic review - updated to Jin 2020 systematic review global</t>
+  </si>
+  <si>
+    <t>from Chen personal communication - 2020 RMB - 8000-14000 includes PCR test and pre-treatment</t>
+  </si>
+  <si>
+    <t>based on Chen RDT - 3 RMB plus double for processing/overheads changed to Ong personal communication (35 RMB for an ELISA test)</t>
+  </si>
+  <si>
+    <t>PCR testing is 140 RMB</t>
+  </si>
+  <si>
+    <t>Assume 10% of treatment costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ong - $11686 2018 USD staff cost for HIVST, assume same for HCV and rest of costs are for HIV.4781 kits delivered </t>
+  </si>
+  <si>
+    <t>VietnamLow</t>
+  </si>
+  <si>
+    <t>VietnamHigh</t>
+  </si>
+  <si>
+    <t>Des Jarlais 2018 - HaiPhong PWID (Drug Alco Depend 2018)</t>
+  </si>
+  <si>
+    <t>Moles 2020 (72% in DRIVE C) - 66% is cited in DRIVE C protocol with range from other studies in Vietnam https://bmjopen.bmj.com/content/10/11/e039234#ref-17</t>
+  </si>
+  <si>
+    <t>Assume 10% of treatment cost</t>
+  </si>
+  <si>
+    <t>The Due 2020 - 2019 USD - no idea why previous estimate is so low? Drug + monitoring costs. Standard error for drug is 276.9 and for monitoring is 71.1, if want to calculate CI. Subtract estimated cost of PCR test.</t>
+  </si>
+  <si>
+    <t>Assume $10 for CBO incentives per person - peer-led testing</t>
+  </si>
+  <si>
+    <t>Jack's paper - increase bounds so max 80% coverage of NSP</t>
+  </si>
+  <si>
+    <t>GeorgiaOld</t>
+  </si>
+  <si>
+    <t>KenyaOld</t>
+  </si>
+  <si>
+    <t>ChinaOld</t>
+  </si>
+  <si>
+    <t>VietnamOld</t>
   </si>
 </sst>
 </file>
@@ -1068,12 +1140,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1089,13 +1167,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1411,22 +1493,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707EB61A-F669-6B48-8A71-B654C41C6040}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="89" customWidth="1"/>
-    <col min="7" max="12" width="20.6640625" customWidth="1"/>
+    <col min="4" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" customWidth="1"/>
+    <col min="10" max="12" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" customWidth="1"/>
+    <col min="14" max="14" width="59.83203125" customWidth="1"/>
+    <col min="15" max="18" width="20.6640625" customWidth="1"/>
+    <col min="19" max="19" width="70" customWidth="1"/>
+    <col min="20" max="23" width="20.6640625" customWidth="1"/>
+    <col min="24" max="24" width="58.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -1437,37 +1525,73 @@
         <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="E1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F1" t="s">
         <v>238</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>316</v>
+      </c>
+      <c r="H1" t="s">
+        <v>317</v>
+      </c>
+      <c r="I1" t="s">
         <v>239</v>
       </c>
-      <c r="G1" t="s">
-        <v>271</v>
-      </c>
-      <c r="H1" t="s">
-        <v>272</v>
-      </c>
-      <c r="I1" t="s">
-        <v>289</v>
-      </c>
       <c r="J1" t="s">
-        <v>290</v>
+        <v>351</v>
       </c>
       <c r="K1" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="L1" t="s">
-        <v>303</v>
+        <v>325</v>
       </c>
       <c r="M1" t="s">
+        <v>326</v>
+      </c>
+      <c r="N1" t="s">
+        <v>267</v>
+      </c>
+      <c r="O1" t="s">
+        <v>352</v>
+      </c>
+      <c r="P1" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>332</v>
+      </c>
+      <c r="R1" t="s">
+        <v>333</v>
+      </c>
+      <c r="S1" t="s">
+        <v>282</v>
+      </c>
+      <c r="T1" t="s">
+        <v>353</v>
+      </c>
+      <c r="U1" t="s">
+        <v>293</v>
+      </c>
+      <c r="V1" t="s">
+        <v>342</v>
+      </c>
+      <c r="W1" t="s">
+        <v>343</v>
+      </c>
+      <c r="X1" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>150</v>
       </c>
@@ -1484,33 +1608,58 @@
         <f>3720000*0.063</f>
         <v>234360</v>
       </c>
-      <c r="F2" t="s">
-        <v>241</v>
-      </c>
-      <c r="G2">
+      <c r="F2">
+        <v>234200</v>
+      </c>
+      <c r="I2" t="s">
+        <v>318</v>
+      </c>
+      <c r="J2">
         <f>AVERAGE(9750,17150)</f>
         <v>13450</v>
       </c>
-      <c r="H2" t="s">
-        <v>273</v>
-      </c>
-      <c r="I2">
+      <c r="K2">
+        <f>AVERAGE(9750,17150)</f>
+        <v>13450</v>
+      </c>
+      <c r="L2">
+        <v>9750</v>
+      </c>
+      <c r="M2">
+        <v>17150</v>
+      </c>
+      <c r="N2" t="s">
+        <v>349</v>
+      </c>
+      <c r="O2">
         <v>17000</v>
       </c>
-      <c r="J2" t="s">
-        <v>291</v>
-      </c>
-      <c r="K2">
+      <c r="P2">
+        <v>17000</v>
+      </c>
+      <c r="S2" t="s">
+        <v>283</v>
+      </c>
+      <c r="T2">
         <v>5000</v>
       </c>
-      <c r="L2" t="s">
-        <v>304</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="U2">
+        <v>5000</v>
+      </c>
+      <c r="V2">
+        <v>4000</v>
+      </c>
+      <c r="W2">
+        <v>6000</v>
+      </c>
+      <c r="X2" t="s">
+        <v>344</v>
+      </c>
+      <c r="Y2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -1526,29 +1675,65 @@
       <c r="E3">
         <v>0.22700000000000001</v>
       </c>
-      <c r="F3" t="s">
-        <v>240</v>
+      <c r="F3">
+        <v>0.22700000000000001</v>
       </c>
       <c r="G3">
+        <v>0.18</v>
+      </c>
+      <c r="H3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I3" t="s">
+        <v>319</v>
+      </c>
+      <c r="J3">
         <v>0.109</v>
       </c>
-      <c r="H3" t="s">
-        <v>274</v>
-      </c>
-      <c r="I3">
+      <c r="K3">
+        <v>0.1285</v>
+      </c>
+      <c r="L3">
+        <v>0.1067</v>
+      </c>
+      <c r="M3">
+        <v>0.15390000000000001</v>
+      </c>
+      <c r="N3" t="s">
+        <v>327</v>
+      </c>
+      <c r="O3">
         <v>0.01</v>
       </c>
-      <c r="J3" t="s">
-        <v>292</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="P3">
+        <v>0.01</v>
+      </c>
+      <c r="Q3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="R3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="S3" t="s">
+        <v>336</v>
+      </c>
+      <c r="T3" s="1">
         <v>0.6</v>
       </c>
-      <c r="L3" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U3" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="X3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -1564,29 +1749,47 @@
       <c r="E4">
         <v>0.76</v>
       </c>
-      <c r="F4" t="s">
-        <v>242</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="F4">
+        <v>0.76</v>
+      </c>
+      <c r="I4" t="s">
+        <v>240</v>
+      </c>
+      <c r="J4" s="1">
         <v>0.71</v>
       </c>
-      <c r="H4" t="s">
-        <v>287</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="K4" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" t="s">
+        <v>279</v>
+      </c>
+      <c r="O4" s="1">
         <v>0.8</v>
       </c>
-      <c r="J4" t="s">
-        <v>299</v>
-      </c>
-      <c r="K4" s="1">
+      <c r="P4" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" t="s">
+        <v>290</v>
+      </c>
+      <c r="T4" s="1">
         <v>0.7</v>
       </c>
-      <c r="L4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U4" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -1602,30 +1805,50 @@
       <c r="E5" s="1">
         <v>0.80400000000000005</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="F5" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J5" s="1">
         <v>0.77400000000000002</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="K5" s="1">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="O5" s="1">
         <v>0.75</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1">
+      <c r="P5" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1">
         <v>0.84</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="U5" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="Y5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -1641,23 +1864,35 @@
       <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
-        <v>244</v>
-      </c>
-      <c r="G6">
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="H6" t="s">
-        <v>275</v>
-      </c>
-      <c r="I6">
+      <c r="I6" t="s">
+        <v>242</v>
+      </c>
+      <c r="J6">
         <v>5</v>
       </c>
       <c r="K6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" t="s">
+        <v>268</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>5</v>
+      </c>
+      <c r="T6">
+        <v>5</v>
+      </c>
+      <c r="U6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>162</v>
       </c>
@@ -1673,32 +1908,57 @@
       <c r="E7">
         <v>2.66</v>
       </c>
-      <c r="F7" t="s">
-        <v>259</v>
+      <c r="F7">
+        <f>E7*Sheet1!F3/Sheet1!E3</f>
+        <v>2.78908709257133</v>
       </c>
       <c r="G7">
+        <f>1.67*Sheet1!F3/Sheet1!E3</f>
+        <v>1.7510434002233535</v>
+      </c>
+      <c r="H7">
+        <f>4.08*Sheet1!F3/Sheet1!E3</f>
+        <v>4.277998247252266</v>
+      </c>
+      <c r="I7" t="s">
+        <v>320</v>
+      </c>
+      <c r="J7">
         <v>14.55</v>
       </c>
-      <c r="H7" t="s">
-        <v>276</v>
-      </c>
-      <c r="I7">
+      <c r="K7">
+        <f>(J7+5.92)*Sheet1!$F$4/Sheet1!$E$4</f>
+        <v>21.430006105137771</v>
+      </c>
+      <c r="N7" t="s">
+        <v>328</v>
+      </c>
+      <c r="O7">
         <v>1</v>
       </c>
-      <c r="J7" t="s">
-        <v>328</v>
-      </c>
-      <c r="K7" s="5">
+      <c r="P7">
+        <f>35/6.91</f>
+        <v>5.0651230101302458</v>
+      </c>
+      <c r="S7" t="s">
+        <v>338</v>
+      </c>
+      <c r="T7" s="5">
         <v>2.2200000000000002</v>
       </c>
-      <c r="L7" t="s">
-        <v>315</v>
-      </c>
-      <c r="M7" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U7" s="5">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" t="s">
+        <v>303</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -1714,29 +1974,52 @@
       <c r="E8">
         <v>26.53</v>
       </c>
-      <c r="F8" t="s">
-        <v>259</v>
-      </c>
-      <c r="G8">
+      <c r="F8">
+        <f>E8*Sheet1!F3/Sheet1!E3</f>
+        <v>27.81747389696142</v>
+      </c>
+      <c r="G8" s="5">
+        <f>F8-1.96*(0.1*E8)</f>
+        <v>22.61759389696142</v>
+      </c>
+      <c r="H8" s="5">
+        <f>F8+1.96*(0.1*E8)</f>
+        <v>33.017353896961424</v>
+      </c>
+      <c r="I8" t="s">
+        <v>321</v>
+      </c>
+      <c r="J8">
         <v>78.5</v>
       </c>
-      <c r="H8" t="s">
-        <v>276</v>
-      </c>
-      <c r="I8">
+      <c r="K8">
+        <f>(J8+20.42)*Sheet1!$F$4/Sheet1!$E$4</f>
+        <v>103.55916970787631</v>
+      </c>
+      <c r="N8" t="s">
+        <v>329</v>
+      </c>
+      <c r="O8">
         <v>50</v>
       </c>
-      <c r="J8" t="s">
-        <v>246</v>
-      </c>
-      <c r="K8">
+      <c r="P8">
+        <f>140/6.91</f>
+        <v>20.260492040520983</v>
+      </c>
+      <c r="S8" t="s">
+        <v>339</v>
+      </c>
+      <c r="T8">
         <v>26</v>
       </c>
-      <c r="L8" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U8">
+        <v>26</v>
+      </c>
+      <c r="X8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -1752,29 +2035,53 @@
       <c r="E9">
         <v>285</v>
       </c>
-      <c r="F9" t="s">
-        <v>263</v>
-      </c>
-      <c r="G9">
+      <c r="F9">
+        <f>E9*Sheet1!$F$3/Sheet1!$D$3</f>
+        <v>306.64591557085947</v>
+      </c>
+      <c r="I9" t="s">
+        <v>324</v>
+      </c>
+      <c r="J9">
         <v>1552</v>
       </c>
-      <c r="H9" t="s">
-        <v>276</v>
-      </c>
-      <c r="I9">
+      <c r="K9">
+        <f>(J9*Sheet1!$F$4/Sheet1!$E$4)-K13</f>
+        <v>1501.4928019624692</v>
+      </c>
+      <c r="N9" t="s">
+        <v>330</v>
+      </c>
+      <c r="O9">
         <v>2247</v>
       </c>
-      <c r="J9" t="s">
-        <v>327</v>
-      </c>
-      <c r="K9">
+      <c r="P9">
+        <f>AVERAGE(Q9:R9)</f>
+        <v>1414.6353111432704</v>
+      </c>
+      <c r="Q9">
+        <f>8000/6.91-P8-P13</f>
+        <v>980.48191027496364</v>
+      </c>
+      <c r="R9">
+        <f>14000/6.91-P8-P13</f>
+        <v>1848.7887120115772</v>
+      </c>
+      <c r="S9" t="s">
+        <v>337</v>
+      </c>
+      <c r="T9">
         <v>122</v>
       </c>
-      <c r="L9" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U9" s="5">
+        <f>1384.4+355.6-U8-U13</f>
+        <v>1542.6</v>
+      </c>
+      <c r="X9" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>160</v>
       </c>
@@ -1790,29 +2097,41 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" t="s">
-        <v>321</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>322</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>323</v>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>309</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>310</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
+        <v>311</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="X10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -1828,23 +2147,35 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" t="s">
-        <v>260</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>279</v>
-      </c>
-      <c r="I11">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>256</v>
+      </c>
+      <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>272</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -1860,20 +2191,32 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="I12">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="M12" t="s">
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>158</v>
       </c>
@@ -1889,23 +2232,43 @@
       <c r="E13">
         <v>38</v>
       </c>
-      <c r="F13" t="s">
-        <v>262</v>
-      </c>
-      <c r="G13">
+      <c r="F13">
+        <f>E13*Sheet1!$F$3/Sheet1!$D$3</f>
+        <v>40.886122076114589</v>
+      </c>
+      <c r="I13" t="s">
+        <v>258</v>
+      </c>
+      <c r="J13">
         <v>59</v>
       </c>
-      <c r="H13" t="s">
-        <v>276</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
       <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <f>(59.29+58.48)*Sheet1!$F$4/Sheet1!$E$4</f>
+        <v>123.29320073288105</v>
+      </c>
+      <c r="N13" t="s">
+        <v>331</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>157</v>
+      </c>
+      <c r="S13" t="s">
+        <v>340</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>171.4</v>
+      </c>
+      <c r="X13" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>167</v>
       </c>
@@ -1922,32 +2285,53 @@
         <f>29465/E2</f>
         <v>0.12572537975763781</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="F14" s="1">
+        <f>29465/F2</f>
+        <v>0.12581127241673784</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="J14" s="1">
         <v>0.5</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="K14" s="1">
         <v>0.5</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y14" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>153</v>
       </c>
@@ -1963,28 +2347,48 @@
       <c r="E15" s="1">
         <v>0.1</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G15" s="1">
+      <c r="F15" s="1">
         <v>0.1</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="J15" s="1">
         <v>0.1</v>
       </c>
-      <c r="J15" s="1"/>
       <c r="K15" s="1">
         <v>0.1</v>
       </c>
       <c r="L15" s="1"/>
-      <c r="M15" t="s">
+      <c r="M15" s="1"/>
+      <c r="N15" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>152</v>
       </c>
@@ -2000,28 +2404,48 @@
       <c r="E16" s="1">
         <v>0.05</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="G16" s="1">
+      <c r="F16" s="1">
         <v>0.05</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="I16" s="1">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="J16" s="1">
         <v>0.05</v>
       </c>
-      <c r="J16" s="1"/>
       <c r="K16" s="1">
         <v>0.05</v>
       </c>
       <c r="L16" s="1"/>
-      <c r="M16" t="s">
+      <c r="M16" s="1"/>
+      <c r="N16" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>168</v>
       </c>
@@ -2038,32 +2462,53 @@
         <f>111322/137727</f>
         <v>0.80828014840953477</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G17" s="1">
+      <c r="F17" s="1">
+        <f>111322/137727</f>
+        <v>0.80828014840953477</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J17" s="1">
         <v>0.99</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>301</v>
       </c>
       <c r="K17" s="1">
         <v>1</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="M17" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="T17" s="1">
+        <v>1</v>
+      </c>
+      <c r="U17" s="1">
+        <v>1</v>
+      </c>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>169</v>
       </c>
@@ -2079,25 +2524,45 @@
       <c r="E18" s="1">
         <v>0.9</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="G18" s="1">
+      <c r="F18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="J18" s="1">
         <v>0.92</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1">
+      <c r="K18" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1">
         <v>0.9</v>
       </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1">
+      <c r="P18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1">
         <v>0.88700000000000001</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U18" s="1">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>156</v>
       </c>
@@ -2113,30 +2578,50 @@
       <c r="E19" s="1">
         <v>0.9</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G19" s="1">
+      <c r="F19" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J19" s="1">
         <v>0.92</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="I19" s="1">
+      <c r="K19" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="O19" s="1">
         <v>0.9</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1">
+      <c r="P19" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1">
         <v>0.96</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="M19" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U19" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -2153,25 +2638,46 @@
         <f>98.9%*(1-E21)</f>
         <v>0.74175000000000013</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G20" s="1">
+      <c r="F20" s="1">
+        <f>98.9%*(1-F21)</f>
+        <v>0.74175000000000013</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J20" s="1">
         <v>0.94799999999999995</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1">
+      <c r="K20" s="1">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1">
         <v>0.98399999999999999</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1">
+      <c r="P20" s="1">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1">
         <v>0.92</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U20" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -2187,25 +2693,45 @@
       <c r="E21" s="1">
         <v>0.25</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G21" s="1">
+      <c r="F21" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J21" s="1">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1"/>
       <c r="K21" s="1">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1">
         <v>0.05</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U21" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>170</v>
       </c>
@@ -2221,20 +2747,36 @@
       <c r="E22" s="1">
         <v>0</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="K22" s="1">
-        <v>0</v>
-      </c>
-      <c r="M22" t="s">
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="T22" s="1">
+        <v>0</v>
+      </c>
+      <c r="U22" s="1">
+        <v>0</v>
+      </c>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="Y22" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>171</v>
       </c>
@@ -2250,24 +2792,44 @@
       <c r="E23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1">
+      <c r="F23" s="1">
         <v>1</v>
       </c>
+      <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1">
         <v>1</v>
       </c>
-      <c r="J23" s="1"/>
       <c r="K23" s="1">
         <v>1</v>
       </c>
       <c r="L23" s="1"/>
-      <c r="M23" t="s">
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1">
+        <v>1</v>
+      </c>
+      <c r="P23" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1">
+        <v>1</v>
+      </c>
+      <c r="U23" s="1">
+        <v>1</v>
+      </c>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>172</v>
       </c>
@@ -2283,32 +2845,52 @@
       <c r="E24" s="1">
         <v>0.92</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G24" s="1">
+      <c r="F24" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="J24" s="1">
         <v>0.9</v>
       </c>
-      <c r="H24" t="s">
-        <v>288</v>
-      </c>
-      <c r="I24" s="1">
+      <c r="K24" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" t="s">
+        <v>280</v>
+      </c>
+      <c r="O24" s="1">
         <v>0.96</v>
       </c>
-      <c r="J24" t="s">
-        <v>298</v>
-      </c>
-      <c r="K24" s="1">
+      <c r="P24" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" t="s">
+        <v>289</v>
+      </c>
+      <c r="T24" s="1">
         <v>0.46</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="M24" t="s">
+      <c r="U24" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="Y24" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>173</v>
       </c>
@@ -2324,34 +2906,54 @@
       <c r="E25" s="1">
         <v>0.98</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G25" s="1">
+      <c r="F25" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J25" s="1">
         <v>0.92</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="I25" s="1">
+      <c r="K25" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="O25" s="1">
         <v>0.96</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="K25" s="1">
+      <c r="P25" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="T25" s="1">
         <v>0.84</v>
       </c>
-      <c r="L25" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="M25" t="s">
+      <c r="U25" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="Y25" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="B26" t="s">
         <v>181</v>
@@ -2365,33 +2967,53 @@
       <c r="E26" s="1">
         <v>0.99</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="G26" s="1">
+      <c r="F26" s="1">
         <v>0.99</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I26" s="1">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J26" s="1">
         <v>0.99</v>
       </c>
-      <c r="J26" s="1"/>
       <c r="K26" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="O26" s="1">
         <v>0.99</v>
       </c>
-      <c r="L26" s="1"/>
-      <c r="M26" t="s">
+      <c r="P26" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="U26" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="102" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>175</v>
       </c>
       <c r="B27" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C27" t="s">
         <v>102</v>
@@ -2402,27 +3024,51 @@
       <c r="E27" s="4">
         <v>0</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="G27" s="4">
+      <c r="F27" s="4">
+        <v>3</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="J27" s="4">
         <v>14.12</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="I27" s="5">
+      <c r="K27" s="4">
+        <f>J27*Sheet1!F4/Sheet1!D4</f>
+        <v>15.475461206654222</v>
+      </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="O27" s="5">
         <v>0.18</v>
       </c>
-      <c r="J27" s="1"/>
-      <c r="K27" s="5">
+      <c r="P27" s="5">
+        <f>11686/4781*Sheet1!F2/Sheet1!E2</f>
+        <v>2.5151233414560719</v>
+      </c>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="T27" s="5">
         <v>1</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U27" s="5">
+        <v>10</v>
+      </c>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>229</v>
       </c>
@@ -2438,26 +3084,47 @@
       <c r="E28" s="1">
         <v>0.7</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1">
+      <c r="F28" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1">
         <v>0.8</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="I28" s="1">
+      <c r="K28" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="O28" s="1">
         <f>4633/4781</f>
         <v>0.96904413302656345</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="K28" s="1">
+      <c r="P28" s="1">
+        <f>4633/4781</f>
+        <v>0.96904413302656345</v>
+      </c>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="T28" s="1">
         <v>0.9</v>
       </c>
-      <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U28" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>231</v>
       </c>
@@ -2473,24 +3140,45 @@
       <c r="E29" s="1">
         <v>0.05</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1">
+      <c r="F29" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1">
         <v>0.8</v>
       </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1">
-        <f t="shared" ref="I29:I30" si="0">4633/4781</f>
+      <c r="K29" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1">
+        <f t="shared" ref="O29:P30" si="0">4633/4781</f>
         <v>0.96904413302656345</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="K29" s="1">
+      <c r="P29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.96904413302656345</v>
+      </c>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="T29" s="1">
         <v>0.05</v>
       </c>
-      <c r="L29" s="1"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U29" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>233</v>
       </c>
@@ -2506,31 +3194,52 @@
       <c r="E30" s="1">
         <v>0.7</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1">
+      <c r="F30" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1">
         <v>0.8</v>
       </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1">
+      <c r="K30" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1">
         <f t="shared" si="0"/>
         <v>0.96904413302656345</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="K30" s="1">
+      <c r="P30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.96904413302656345</v>
+      </c>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="T30" s="1">
         <v>0.5</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U30" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B31" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C31" t="s">
         <v>102</v>
@@ -2541,13 +3250,36 @@
       <c r="E31">
         <v>26.53</v>
       </c>
-      <c r="G31">
+      <c r="F31">
+        <f>E31*Sheet1!F3/Sheet1!E3</f>
+        <v>27.81747389696142</v>
+      </c>
+      <c r="G31" s="5">
+        <f>F31-1.96*(0.1*E31)</f>
+        <v>22.61759389696142</v>
+      </c>
+      <c r="H31" s="5">
+        <f>F31+1.96*(0.1*E31)</f>
+        <v>33.017353896961424</v>
+      </c>
+      <c r="J31">
         <v>78.5</v>
       </c>
-      <c r="I31">
+      <c r="K31">
+        <f>K8</f>
+        <v>103.55916970787631</v>
+      </c>
+      <c r="O31">
         <v>50</v>
       </c>
-      <c r="K31">
+      <c r="P31">
+        <f>P8</f>
+        <v>20.260492040520983</v>
+      </c>
+      <c r="T31">
+        <v>26</v>
+      </c>
+      <c r="U31">
         <v>26</v>
       </c>
     </row>
@@ -2557,6 +3289,125 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE11F68-A115-1B46-B2E0-B5D7701E800A}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B1">
+        <v>2015</v>
+      </c>
+      <c r="C1">
+        <v>2016</v>
+      </c>
+      <c r="D1">
+        <v>2017</v>
+      </c>
+      <c r="E1">
+        <v>2018</v>
+      </c>
+      <c r="F1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B2">
+        <v>114.92212455459099</v>
+      </c>
+      <c r="C2">
+        <v>117.220567045682</v>
+      </c>
+      <c r="D2">
+        <v>119.088051569694</v>
+      </c>
+      <c r="E2">
+        <v>121.558877247618</v>
+      </c>
+      <c r="F2">
+        <v>125.083155733959</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3">
+        <v>114.664725</v>
+      </c>
+      <c r="C3">
+        <v>117.112733333333</v>
+      </c>
+      <c r="D3">
+        <v>124.18085833333301</v>
+      </c>
+      <c r="E3">
+        <v>127.428491666667</v>
+      </c>
+      <c r="F3">
+        <v>133.61246666666699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B4">
+        <v>150.18963879765201</v>
+      </c>
+      <c r="C4">
+        <v>159.647316938312</v>
+      </c>
+      <c r="D4">
+        <v>172.42823857621599</v>
+      </c>
+      <c r="E4">
+        <v>180.514812183022</v>
+      </c>
+      <c r="F4" s="6">
+        <f>E4/D4*E4</f>
+        <v>188.98063151685196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B5">
+        <v>144.55037019428801</v>
+      </c>
+      <c r="C5">
+        <v>148.40733280127799</v>
+      </c>
+      <c r="D5">
+        <v>153.63165215668499</v>
+      </c>
+      <c r="E5">
+        <v>159.06964122458299</v>
+      </c>
+      <c r="F5">
+        <v>163.516947912918</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D1F24D-5226-E34A-88F5-702AF231CD7B}">
   <dimension ref="A1:I67"/>
   <sheetViews>
@@ -2623,7 +3474,7 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="H2" s="1">
         <v>0.2</v>
@@ -2652,7 +3503,7 @@
         <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="H3" s="1">
         <v>0.7</v>
@@ -2669,7 +3520,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -2681,7 +3532,7 @@
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="H4" s="1">
         <v>0.1</v>
@@ -3074,7 +3925,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -3092,12 +3943,12 @@
         <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B20">
         <v>20</v>
@@ -3109,16 +3960,16 @@
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F20" t="s">
         <v>100</v>
       </c>
       <c r="G20" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="I20" t="s">
         <v>180</v>
@@ -3126,7 +3977,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -3144,15 +3995,15 @@
         <v>100</v>
       </c>
       <c r="G21" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B22">
         <v>20</v>
@@ -3164,21 +4015,21 @@
         <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F22" t="s">
         <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B23">
         <v>20</v>
@@ -3196,10 +4047,10 @@
         <v>100</v>
       </c>
       <c r="G23" t="s">
+        <v>259</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="I23" t="s">
         <v>116</v>
@@ -4381,7 +5232,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9501918-23E8-1749-856B-118F67DC083D}">
   <dimension ref="A1:F73"/>
   <sheetViews>

</xml_diff>

<commit_message>
update model structure and parameters to use sens and spec
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FB2739-89C7-1F47-8AAF-D50E4BC0FA80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D6EE5D-55AE-3F4E-BB1D-D1DAA6A42188}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" activeTab="2" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="378">
   <si>
     <t>NumberFrom</t>
   </si>
@@ -472,9 +472,6 @@
     <t>Calculate based on how many have been treated? This is % antibody tests that get chronic result.</t>
   </si>
   <si>
-    <t>AntibodyReTestPos</t>
-  </si>
-  <si>
     <t>Vary this in first sensitivity analysis</t>
   </si>
   <si>
@@ -1013,9 +1010,6 @@
   </si>
   <si>
     <t>2019 not available</t>
-  </si>
-  <si>
-    <t>LIFER study - removed pre treatment stuff from 338 total - 2017 USD</t>
   </si>
   <si>
     <t>KenyaLow</t>
@@ -1105,13 +1099,91 @@
   </si>
   <si>
     <t>VietnamOld</t>
+  </si>
+  <si>
+    <t>sens</t>
+  </si>
+  <si>
+    <t>OraQuick sensitivity</t>
+  </si>
+  <si>
+    <t>spec</t>
+  </si>
+  <si>
+    <t>OraQuick specificity</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>RDTCost</t>
+  </si>
+  <si>
+    <t>LIFER study - removed pre treatment stuff from 338 total - 2017 USD. Should be 767 total?</t>
+  </si>
+  <si>
+    <t>sens2</t>
+  </si>
+  <si>
+    <t>spec2</t>
+  </si>
+  <si>
+    <t>Retest sensitivity</t>
+  </si>
+  <si>
+    <t>Retest specificity</t>
+  </si>
+  <si>
+    <t>NewModel</t>
+  </si>
+  <si>
+    <t>b*(sens2 + (1-spec2))</t>
+  </si>
+  <si>
+    <t>1 - b*(sens2 + (1-spec2))</t>
+  </si>
+  <si>
+    <t>d*sens2/(sens2 + (1-spec2))</t>
+  </si>
+  <si>
+    <t>1 - d*sens2/(sens2 + (1-spec2))</t>
+  </si>
+  <si>
+    <t>v*w*z1*b*(sens*x + (1-spec*x))</t>
+  </si>
+  <si>
+    <t>(1-v)*w*z1*b*(sens*x + (1-spec*x))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> w*z2*(1-b*(sens*x + (1-spec*x)))</t>
+  </si>
+  <si>
+    <t>d*sens*x/(sens*x + (1 - spec*x))</t>
+  </si>
+  <si>
+    <t>1 - d*sens*x/(sens*x + (1 - spec*x))</t>
+  </si>
+  <si>
+    <t>[sens*sens2*x + (1-spec*x)*(1-spec2)] / [sens*x + (1-spec*x)]</t>
+  </si>
+  <si>
+    <t>1 - [sens*sens2*x + (1-spec*x)*(1-spec2)] / [sens*x + (1-spec*x)]</t>
+  </si>
+  <si>
+    <t>Interreaderagreement</t>
+  </si>
+  <si>
+    <t>1 - ytest</t>
+  </si>
+  <si>
+    <t>1-p  this was likely causing strange results before</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1135,6 +1207,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1167,7 +1246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1178,6 +1257,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1493,10 +1574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707EB61A-F669-6B48-8A71-B654C41C6040}">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1516,7 +1597,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
         <v>97</v>
@@ -1525,67 +1606,67 @@
         <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E1" t="s">
+        <v>348</v>
+      </c>
+      <c r="F1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1" t="s">
+        <v>315</v>
+      </c>
+      <c r="H1" t="s">
+        <v>316</v>
+      </c>
+      <c r="I1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J1" t="s">
+        <v>349</v>
+      </c>
+      <c r="K1" t="s">
+        <v>265</v>
+      </c>
+      <c r="L1" t="s">
+        <v>323</v>
+      </c>
+      <c r="M1" t="s">
+        <v>324</v>
+      </c>
+      <c r="N1" t="s">
+        <v>266</v>
+      </c>
+      <c r="O1" t="s">
         <v>350</v>
       </c>
-      <c r="F1" t="s">
-        <v>238</v>
-      </c>
-      <c r="G1" t="s">
-        <v>316</v>
-      </c>
-      <c r="H1" t="s">
-        <v>317</v>
-      </c>
-      <c r="I1" t="s">
-        <v>239</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="P1" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>330</v>
+      </c>
+      <c r="R1" t="s">
+        <v>331</v>
+      </c>
+      <c r="S1" t="s">
+        <v>281</v>
+      </c>
+      <c r="T1" t="s">
         <v>351</v>
       </c>
-      <c r="K1" t="s">
-        <v>266</v>
-      </c>
-      <c r="L1" t="s">
-        <v>325</v>
-      </c>
-      <c r="M1" t="s">
-        <v>326</v>
-      </c>
-      <c r="N1" t="s">
-        <v>267</v>
-      </c>
-      <c r="O1" t="s">
-        <v>352</v>
-      </c>
-      <c r="P1" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>332</v>
-      </c>
-      <c r="R1" t="s">
-        <v>333</v>
-      </c>
-      <c r="S1" t="s">
-        <v>282</v>
-      </c>
-      <c r="T1" t="s">
-        <v>353</v>
-      </c>
       <c r="U1" t="s">
+        <v>292</v>
+      </c>
+      <c r="V1" t="s">
+        <v>340</v>
+      </c>
+      <c r="W1" t="s">
+        <v>341</v>
+      </c>
+      <c r="X1" t="s">
         <v>293</v>
-      </c>
-      <c r="V1" t="s">
-        <v>342</v>
-      </c>
-      <c r="W1" t="s">
-        <v>343</v>
-      </c>
-      <c r="X1" t="s">
-        <v>294</v>
       </c>
       <c r="Y1" t="s">
         <v>106</v>
@@ -1593,7 +1674,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
         <v>98</v>
@@ -1612,7 +1693,7 @@
         <v>234200</v>
       </c>
       <c r="I2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J2">
         <f>AVERAGE(9750,17150)</f>
@@ -1629,7 +1710,7 @@
         <v>17150</v>
       </c>
       <c r="N2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="O2">
         <v>17000</v>
@@ -1638,7 +1719,7 @@
         <v>17000</v>
       </c>
       <c r="S2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="T2">
         <v>5000</v>
@@ -1653,15 +1734,15 @@
         <v>6000</v>
       </c>
       <c r="X2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="Y2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>110</v>
@@ -1679,13 +1760,13 @@
         <v>0.22700000000000001</v>
       </c>
       <c r="G3">
-        <v>0.18</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="H3">
-        <v>0.28000000000000003</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="I3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J3">
         <v>0.109</v>
@@ -1700,7 +1781,7 @@
         <v>0.15390000000000001</v>
       </c>
       <c r="N3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="O3">
         <v>0.01</v>
@@ -1715,7 +1796,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="S3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="T3" s="1">
         <v>0.6</v>
@@ -1730,12 +1811,12 @@
         <v>0.87</v>
       </c>
       <c r="X3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
         <v>104</v>
@@ -1753,7 +1834,7 @@
         <v>0.76</v>
       </c>
       <c r="I4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J4" s="1">
         <v>0.71</v>
@@ -1764,7 +1845,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O4" s="1">
         <v>0.8</v>
@@ -1775,7 +1856,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="T4" s="1">
         <v>0.7</v>
@@ -1786,12 +1867,12 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
         <v>130</v>
@@ -1811,7 +1892,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J5" s="1">
         <v>0.77400000000000002</v>
@@ -1822,7 +1903,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O5" s="1">
         <v>0.75</v>
@@ -1842,7 +1923,7 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Y5" t="s">
         <v>142</v>
@@ -1850,7 +1931,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
         <v>124</v>
@@ -1868,7 +1949,7 @@
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J6">
         <v>5</v>
@@ -1877,7 +1958,7 @@
         <v>5</v>
       </c>
       <c r="N6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O6">
         <v>5</v>
@@ -1894,7 +1975,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s">
         <v>121</v>
@@ -1906,32 +1987,21 @@
         <v>10</v>
       </c>
       <c r="E7">
-        <v>2.66</v>
+        <v>31.24</v>
       </c>
       <c r="F7">
         <f>E7*Sheet1!F3/Sheet1!E3</f>
-        <v>2.78908709257133</v>
-      </c>
-      <c r="G7">
-        <f>1.67*Sheet1!F3/Sheet1!E3</f>
-        <v>1.7510434002233535</v>
-      </c>
-      <c r="H7">
-        <f>4.08*Sheet1!F3/Sheet1!E3</f>
-        <v>4.277998247252266</v>
+        <v>32.756045402980575</v>
       </c>
       <c r="I7" t="s">
-        <v>320</v>
-      </c>
-      <c r="J7">
-        <v>14.55</v>
+        <v>319</v>
       </c>
       <c r="K7">
-        <f>(J7+5.92)*Sheet1!$F$4/Sheet1!$E$4</f>
-        <v>21.430006105137771</v>
+        <f>K34*2</f>
+        <v>42.860012210275542</v>
       </c>
       <c r="N7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -1941,26 +2011,24 @@
         <v>5.0651230101302458</v>
       </c>
       <c r="S7" t="s">
-        <v>338</v>
-      </c>
-      <c r="T7" s="5">
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="U7" s="5">
-        <v>2.2200000000000002</v>
+        <v>336</v>
+      </c>
+      <c r="U7">
+        <f>U34*2</f>
+        <v>4.4400000000000004</v>
       </c>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Y7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
         <v>122</v>
@@ -1987,7 +2055,7 @@
         <v>33.017353896961424</v>
       </c>
       <c r="I8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J8">
         <v>78.5</v>
@@ -1997,7 +2065,7 @@
         <v>103.55916970787631</v>
       </c>
       <c r="N8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="O8">
         <v>50</v>
@@ -2007,7 +2075,7 @@
         <v>20.260492040520983</v>
       </c>
       <c r="S8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="T8">
         <v>26</v>
@@ -2016,12 +2084,12 @@
         <v>26</v>
       </c>
       <c r="X8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
         <v>123</v>
@@ -2033,14 +2101,15 @@
         <v>200</v>
       </c>
       <c r="E9">
-        <v>285</v>
+        <f>767-E13</f>
+        <v>729</v>
       </c>
       <c r="F9">
         <f>E9*Sheet1!$F$3/Sheet1!$D$3</f>
-        <v>306.64591557085947</v>
+        <v>784.36797351282996</v>
       </c>
       <c r="I9" t="s">
-        <v>324</v>
+        <v>358</v>
       </c>
       <c r="J9">
         <v>1552</v>
@@ -2050,7 +2119,7 @@
         <v>1501.4928019624692</v>
       </c>
       <c r="N9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="O9">
         <v>2247</v>
@@ -2068,7 +2137,7 @@
         <v>1848.7887120115772</v>
       </c>
       <c r="S9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="T9">
         <v>122</v>
@@ -2078,15 +2147,15 @@
         <v>1542.6</v>
       </c>
       <c r="X9" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C10" t="s">
         <v>102</v>
@@ -2101,42 +2170,42 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
+        <v>308</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
         <v>309</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
         <v>310</v>
       </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="S10" t="s">
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="X10" t="s">
         <v>311</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="X10" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C11" t="s">
         <v>102</v>
@@ -2151,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -2160,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -2177,10 +2246,10 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
         <v>102</v>
@@ -2218,10 +2287,10 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C13" t="s">
         <v>102</v>
@@ -2237,7 +2306,7 @@
         <v>40.886122076114589</v>
       </c>
       <c r="I13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J13">
         <v>59</v>
@@ -2247,7 +2316,7 @@
         <v>123.29320073288105</v>
       </c>
       <c r="N13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -2256,7 +2325,7 @@
         <v>157</v>
       </c>
       <c r="S13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="T13">
         <v>0</v>
@@ -2265,12 +2334,12 @@
         <v>171.4</v>
       </c>
       <c r="X13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B14" t="s">
         <v>127</v>
@@ -2292,7 +2361,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J14" s="1">
         <v>0.5</v>
@@ -2303,7 +2372,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O14" s="1">
         <v>0.1</v>
@@ -2314,7 +2383,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="T14" s="1">
         <v>0.5</v>
@@ -2325,15 +2394,15 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Y14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B15" t="s">
         <v>128</v>
@@ -2353,7 +2422,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J15" s="1">
         <v>0.1</v>
@@ -2364,7 +2433,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O15" s="1">
         <v>0.1</v>
@@ -2385,12 +2454,12 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
         <v>129</v>
@@ -2410,7 +2479,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J16" s="1">
         <v>0.05</v>
@@ -2421,7 +2490,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O16" s="1">
         <v>0.05</v>
@@ -2442,12 +2511,12 @@
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
         <v>131</v>
@@ -2469,7 +2538,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J17" s="1">
         <v>0.99</v>
@@ -2480,7 +2549,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O17" s="1">
         <v>0.9</v>
@@ -2491,7 +2560,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T17" s="1">
         <v>1</v>
@@ -2502,15 +2571,15 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="Y17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
         <v>132</v>
@@ -2530,7 +2599,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J18" s="1">
         <v>0.92</v>
@@ -2559,12 +2628,12 @@
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B19" t="s">
         <v>133</v>
@@ -2584,7 +2653,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J19" s="1">
         <v>0.92</v>
@@ -2595,7 +2664,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O19" s="1">
         <v>0.9</v>
@@ -2615,15 +2684,15 @@
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="Y19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20" t="s">
         <v>134</v>
@@ -2645,7 +2714,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J20" s="1">
         <v>0.94799999999999995</v>
@@ -2674,12 +2743,12 @@
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B21" t="s">
         <v>135</v>
@@ -2699,7 +2768,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J21" s="1">
         <v>2.5000000000000001E-4</v>
@@ -2728,12 +2797,12 @@
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B22" t="s">
         <v>136</v>
@@ -2778,7 +2847,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B23" t="s">
         <v>139</v>
@@ -2826,12 +2895,12 @@
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
         <v>141</v>
@@ -2846,56 +2915,56 @@
         <v>0.92</v>
       </c>
       <c r="F24" s="1">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J24" s="1">
         <v>0.9</v>
       </c>
       <c r="K24" s="1">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O24" s="1">
         <v>0.96</v>
       </c>
       <c r="P24" s="1">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T24" s="1">
         <v>0.46</v>
       </c>
       <c r="U24" s="1">
-        <v>0.46</v>
+        <v>0.95</v>
       </c>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Y24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>375</v>
       </c>
       <c r="C25" t="s">
         <v>126</v>
@@ -2912,51 +2981,51 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J25" s="1">
         <v>0.92</v>
       </c>
       <c r="K25" s="1">
-        <v>0.92</v>
+        <v>0.97</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O25" s="1">
         <v>0.96</v>
       </c>
       <c r="P25" s="1">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="T25" s="1">
         <v>0.84</v>
       </c>
       <c r="U25" s="1">
-        <v>0.84</v>
+        <v>0.88</v>
       </c>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Y25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C26" t="s">
         <v>125</v>
@@ -2968,29 +3037,29 @@
         <v>0.99</v>
       </c>
       <c r="F26" s="1">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J26" s="1">
         <v>0.99</v>
       </c>
       <c r="K26" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O26" s="1">
         <v>0.99</v>
       </c>
       <c r="P26" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -2999,21 +3068,21 @@
         <v>0.99</v>
       </c>
       <c r="U26" s="1">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
       <c r="Y26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="102" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B27" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C27" t="s">
         <v>102</v>
@@ -3030,7 +3099,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="J27" s="4">
         <v>14.12</v>
@@ -3042,7 +3111,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="O27" s="5">
         <v>0.18</v>
@@ -3054,7 +3123,7 @@
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
       <c r="S27" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="T27" s="5">
         <v>1</v>
@@ -3065,15 +3134,15 @@
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
       <c r="X27" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C28" t="s">
         <v>125</v>
@@ -3085,7 +3154,7 @@
         <v>0.7</v>
       </c>
       <c r="F28" s="1">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -3099,26 +3168,25 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O28" s="1">
         <f>4633/4781</f>
         <v>0.96904413302656345</v>
       </c>
       <c r="P28" s="1">
-        <f>4633/4781</f>
-        <v>0.96904413302656345</v>
+        <v>0.65</v>
       </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="T28" s="1">
         <v>0.9</v>
       </c>
       <c r="U28" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
@@ -3126,10 +3194,10 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C29" t="s">
         <v>125</v>
@@ -3150,7 +3218,7 @@
         <v>0.8</v>
       </c>
       <c r="K29" s="1">
-        <v>0.8</v>
+        <v>0.05</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -3160,13 +3228,12 @@
         <v>0.96904413302656345</v>
       </c>
       <c r="P29" s="1">
-        <f t="shared" si="0"/>
-        <v>0.96904413302656345</v>
+        <v>0.05</v>
       </c>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T29" s="1">
         <v>0.05</v>
@@ -3180,10 +3247,10 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C30" t="s">
         <v>125</v>
@@ -3195,7 +3262,7 @@
         <v>0.7</v>
       </c>
       <c r="F30" s="1">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -3214,32 +3281,31 @@
         <v>0.96904413302656345</v>
       </c>
       <c r="P30" s="1">
-        <f t="shared" si="0"/>
-        <v>0.96904413302656345</v>
+        <v>0.65</v>
       </c>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T30" s="1">
         <v>0.5</v>
       </c>
       <c r="U30" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>313</v>
+      </c>
+      <c r="B31" t="s">
         <v>314</v>
-      </c>
-      <c r="B31" t="s">
-        <v>315</v>
       </c>
       <c r="C31" t="s">
         <v>102</v>
@@ -3281,6 +3347,144 @@
       </c>
       <c r="U31">
         <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>352</v>
+      </c>
+      <c r="B32" t="s">
+        <v>353</v>
+      </c>
+      <c r="C32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="G32">
+        <v>0.97</v>
+      </c>
+      <c r="H32">
+        <v>0.99</v>
+      </c>
+      <c r="K32" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="P32" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="U32" s="8">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>354</v>
+      </c>
+      <c r="B33" t="s">
+        <v>355</v>
+      </c>
+      <c r="C33" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" s="8">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>0.9</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="K33" s="8">
+        <v>1</v>
+      </c>
+      <c r="P33" s="8">
+        <v>1</v>
+      </c>
+      <c r="U33" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>356</v>
+      </c>
+      <c r="B34" t="s">
+        <v>357</v>
+      </c>
+      <c r="E34">
+        <v>2.66</v>
+      </c>
+      <c r="F34">
+        <f>E34*Sheet1!F3/Sheet1!E3</f>
+        <v>2.78908709257133</v>
+      </c>
+      <c r="G34">
+        <f>1.67*Sheet1!F3/Sheet1!E3</f>
+        <v>1.7510434002233535</v>
+      </c>
+      <c r="H34">
+        <f>4.08*Sheet1!F3/Sheet1!E3</f>
+        <v>4.277998247252266</v>
+      </c>
+      <c r="J34">
+        <v>14.55</v>
+      </c>
+      <c r="K34">
+        <f>(J34+5.92)*Sheet1!$F$4/Sheet1!$E$4</f>
+        <v>21.430006105137771</v>
+      </c>
+      <c r="P34">
+        <f>6/6.91</f>
+        <v>0.86830680173661356</v>
+      </c>
+      <c r="T34" s="5">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="U34" s="5">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>359</v>
+      </c>
+      <c r="B35" t="s">
+        <v>361</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="U35" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>360</v>
+      </c>
+      <c r="B36" t="s">
+        <v>362</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3300,7 +3504,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B1">
         <v>2015</v>
@@ -3320,7 +3524,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B2">
         <v>114.92212455459099</v>
@@ -3340,7 +3544,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B3">
         <v>114.664725</v>
@@ -3360,7 +3564,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B4">
         <v>150.18963879765201</v>
@@ -3379,12 +3583,12 @@
         <v>188.98063151685196</v>
       </c>
       <c r="G4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B5">
         <v>144.55037019428801</v>
@@ -3409,10 +3613,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D1F24D-5226-E34A-88F5-702AF231CD7B}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3421,11 +3625,12 @@
     <col min="3" max="3" width="29.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
     <col min="6" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.33203125" customWidth="1"/>
-    <col min="9" max="9" width="32.5" customWidth="1"/>
+    <col min="8" max="8" width="34.5" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" customWidth="1"/>
+    <col min="10" max="10" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3448,13 +3653,16 @@
         <v>97</v>
       </c>
       <c r="H1" t="s">
+        <v>363</v>
+      </c>
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -3468,22 +3676,22 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>306</v>
-      </c>
-      <c r="H2" s="1">
+        <v>305</v>
+      </c>
+      <c r="I2" s="1">
         <v>0.2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -3503,16 +3711,16 @@
         <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>307</v>
-      </c>
-      <c r="H3" s="1">
+        <v>306</v>
+      </c>
+      <c r="I3" s="1">
         <v>0.7</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -3520,25 +3728,25 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F4" t="s">
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>308</v>
-      </c>
-      <c r="H4" s="1">
+        <v>307</v>
+      </c>
+      <c r="I4" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3552,19 +3760,22 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F5" t="s">
         <v>100</v>
       </c>
-      <c r="G5" t="s">
-        <v>151</v>
+      <c r="G5" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="H5" t="s">
+        <v>364</v>
+      </c>
+      <c r="I5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3578,19 +3789,22 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F6" t="s">
         <v>100</v>
       </c>
-      <c r="G6" t="s">
-        <v>188</v>
+      <c r="G6" s="9" t="s">
+        <v>187</v>
       </c>
       <c r="H6" t="s">
+        <v>365</v>
+      </c>
+      <c r="I6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3604,22 +3818,22 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F7" t="s">
         <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>168</v>
-      </c>
-      <c r="H7" s="1">
+        <v>167</v>
+      </c>
+      <c r="I7" s="1">
         <v>0.9</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -3639,13 +3853,13 @@
         <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>183</v>
-      </c>
-      <c r="H8" t="s">
+        <v>182</v>
+      </c>
+      <c r="I8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3659,22 +3873,25 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F9" t="s">
         <v>100</v>
       </c>
-      <c r="G9" t="s">
-        <v>154</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="G9" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H9" t="s">
+        <v>366</v>
+      </c>
+      <c r="I9" s="1">
         <v>0.75</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -3688,19 +3905,22 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F10" t="s">
         <v>100</v>
       </c>
-      <c r="G10" t="s">
-        <v>184</v>
+      <c r="G10" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="H10" t="s">
+        <v>367</v>
+      </c>
+      <c r="I10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -3714,22 +3934,22 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F11" t="s">
         <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>169</v>
-      </c>
-      <c r="H11" s="1">
+        <v>168</v>
+      </c>
+      <c r="I11" s="1">
         <v>0.9</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -3749,13 +3969,13 @@
         <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>185</v>
-      </c>
-      <c r="H12" t="s">
+        <v>184</v>
+      </c>
+      <c r="I12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3769,22 +3989,22 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F13" t="s">
         <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>156</v>
-      </c>
-      <c r="H13" s="1">
+        <v>155</v>
+      </c>
+      <c r="I13" s="1">
         <v>0.9</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -3804,13 +4024,13 @@
         <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>186</v>
-      </c>
-      <c r="H14" t="s">
+        <v>185</v>
+      </c>
+      <c r="I14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -3824,19 +4044,19 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F15" t="s">
         <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>157</v>
-      </c>
-      <c r="H15" s="1">
+        <v>156</v>
+      </c>
+      <c r="I15" s="1">
         <v>0.95</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -3850,22 +4070,22 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
       </c>
       <c r="G16" t="s">
-        <v>187</v>
-      </c>
-      <c r="H16" s="1">
+        <v>186</v>
+      </c>
+      <c r="I16" s="1">
         <v>0.03</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -3885,16 +4105,16 @@
         <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>155</v>
-      </c>
-      <c r="H17" t="s">
+        <v>154</v>
+      </c>
+      <c r="I17" t="s">
         <v>113</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -3914,18 +4134,18 @@
         <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>170</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" t="s">
+        <v>169</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -3942,13 +4162,16 @@
       <c r="F19" t="s">
         <v>100</v>
       </c>
-      <c r="G19" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G19" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H19" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B20">
         <v>20</v>
@@ -3960,24 +4183,27 @@
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F20" t="s">
         <v>100</v>
       </c>
-      <c r="G20" t="s">
-        <v>253</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="I20" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G20" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="H20" t="s">
+        <v>368</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -3989,21 +4215,24 @@
         <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F21" t="s">
         <v>100</v>
       </c>
-      <c r="G21" t="s">
-        <v>252</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G21" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="H21" t="s">
+        <v>369</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B22">
         <v>20</v>
@@ -4015,21 +4244,24 @@
         <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F22" t="s">
         <v>100</v>
       </c>
-      <c r="G22" t="s">
-        <v>251</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G22" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="H22" t="s">
+        <v>370</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B23">
         <v>20</v>
@@ -4041,22 +4273,25 @@
         <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F23" t="s">
         <v>100</v>
       </c>
-      <c r="G23" t="s">
-        <v>259</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="G23" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="H23" t="s">
+        <v>258</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J23" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -4075,14 +4310,17 @@
       <c r="F24" t="s">
         <v>100</v>
       </c>
-      <c r="G24" t="s">
-        <v>183</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="G24" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="H24" t="s">
+        <v>376</v>
+      </c>
+      <c r="I24" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -4096,22 +4334,25 @@
         <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F25" t="s">
         <v>100</v>
       </c>
-      <c r="G25" t="s">
-        <v>168</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="G25" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="H25" t="s">
+        <v>312</v>
+      </c>
+      <c r="I25" s="1">
         <v>0.9</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -4125,22 +4366,25 @@
         <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F26" t="s">
         <v>100</v>
       </c>
-      <c r="G26" t="s">
-        <v>154</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="G26" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H26" t="s">
+        <v>371</v>
+      </c>
+      <c r="I26" s="1">
         <v>0.75</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -4154,19 +4398,22 @@
         <v>32</v>
       </c>
       <c r="E27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F27" t="s">
         <v>100</v>
       </c>
-      <c r="G27" t="s">
-        <v>184</v>
+      <c r="G27" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="H27" t="s">
+        <v>372</v>
+      </c>
+      <c r="I27" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -4180,22 +4427,22 @@
         <v>25</v>
       </c>
       <c r="E28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F28" t="s">
         <v>100</v>
       </c>
       <c r="G28" t="s">
-        <v>169</v>
-      </c>
-      <c r="H28" s="1">
+        <v>168</v>
+      </c>
+      <c r="I28" s="1">
         <v>0.9</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -4215,13 +4462,13 @@
         <v>100</v>
       </c>
       <c r="G29" t="s">
-        <v>185</v>
-      </c>
-      <c r="H29" t="s">
+        <v>184</v>
+      </c>
+      <c r="I29" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -4235,22 +4482,22 @@
         <v>26</v>
       </c>
       <c r="E30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F30" t="s">
         <v>100</v>
       </c>
       <c r="G30" t="s">
-        <v>156</v>
-      </c>
-      <c r="H30" s="1">
+        <v>155</v>
+      </c>
+      <c r="I30" s="1">
         <v>0.9</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -4270,13 +4517,13 @@
         <v>100</v>
       </c>
       <c r="G31" t="s">
-        <v>186</v>
-      </c>
-      <c r="H31" t="s">
+        <v>185</v>
+      </c>
+      <c r="I31" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -4290,19 +4537,19 @@
         <v>27</v>
       </c>
       <c r="E32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F32" t="s">
         <v>100</v>
       </c>
       <c r="G32" t="s">
-        <v>157</v>
-      </c>
-      <c r="H32" s="1">
+        <v>156</v>
+      </c>
+      <c r="I32" s="1">
         <v>0.95</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -4316,19 +4563,19 @@
         <v>28</v>
       </c>
       <c r="E33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F33" t="s">
         <v>100</v>
       </c>
       <c r="G33" t="s">
-        <v>187</v>
-      </c>
-      <c r="H33" s="1">
+        <v>186</v>
+      </c>
+      <c r="I33" s="1">
         <v>0.03</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -4348,16 +4595,16 @@
         <v>100</v>
       </c>
       <c r="G34" t="s">
-        <v>155</v>
-      </c>
-      <c r="H34" t="s">
+        <v>154</v>
+      </c>
+      <c r="I34" t="s">
         <v>113</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -4377,13 +4624,13 @@
         <v>100</v>
       </c>
       <c r="G35" t="s">
-        <v>191</v>
-      </c>
-      <c r="H35" s="1">
+        <v>190</v>
+      </c>
+      <c r="I35" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -4397,19 +4644,19 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F36" t="s">
         <v>100</v>
       </c>
       <c r="G36" t="s">
-        <v>174</v>
-      </c>
-      <c r="H36" s="1">
+        <v>173</v>
+      </c>
+      <c r="I36" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -4423,19 +4670,22 @@
         <v>36</v>
       </c>
       <c r="E37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F37" t="s">
         <v>100</v>
       </c>
-      <c r="G37" t="s">
-        <v>173</v>
-      </c>
-      <c r="H37" s="1">
+      <c r="G37" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="H37" t="s">
+        <v>373</v>
+      </c>
+      <c r="I37" s="1">
         <v>0.98</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>64</v>
       </c>
@@ -4449,22 +4699,25 @@
         <v>48</v>
       </c>
       <c r="E38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F38" t="s">
         <v>100</v>
       </c>
-      <c r="G38" t="s">
-        <v>182</v>
-      </c>
-      <c r="H38" s="1">
+      <c r="G38" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H38" t="s">
+        <v>374</v>
+      </c>
+      <c r="I38" s="1">
         <v>0.02</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -4478,19 +4731,19 @@
         <v>37</v>
       </c>
       <c r="E39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F39" t="s">
         <v>100</v>
       </c>
       <c r="G39" t="s">
-        <v>168</v>
-      </c>
-      <c r="H39" s="1">
+        <v>167</v>
+      </c>
+      <c r="I39" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>65</v>
       </c>
@@ -4510,13 +4763,13 @@
         <v>100</v>
       </c>
       <c r="G40" t="s">
-        <v>183</v>
-      </c>
-      <c r="H40" t="s">
+        <v>182</v>
+      </c>
+      <c r="I40" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>67</v>
       </c>
@@ -4530,22 +4783,25 @@
         <v>38</v>
       </c>
       <c r="E41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F41" t="s">
         <v>100</v>
       </c>
-      <c r="G41" t="s">
-        <v>154</v>
-      </c>
-      <c r="H41" s="1">
+      <c r="G41" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H41" t="s">
+        <v>366</v>
+      </c>
+      <c r="I41" s="1">
         <v>0.75</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>67</v>
       </c>
@@ -4559,19 +4815,22 @@
         <v>46</v>
       </c>
       <c r="E42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F42" t="s">
         <v>100</v>
       </c>
-      <c r="G42" t="s">
-        <v>184</v>
+      <c r="G42" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="H42" t="s">
+        <v>367</v>
+      </c>
+      <c r="I42" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -4585,19 +4844,19 @@
         <v>39</v>
       </c>
       <c r="E43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F43" t="s">
         <v>100</v>
       </c>
       <c r="G43" t="s">
-        <v>169</v>
-      </c>
-      <c r="H43" s="1">
+        <v>168</v>
+      </c>
+      <c r="I43" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -4617,13 +4876,13 @@
         <v>100</v>
       </c>
       <c r="G44" t="s">
-        <v>185</v>
-      </c>
-      <c r="H44" t="s">
+        <v>184</v>
+      </c>
+      <c r="I44" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>71</v>
       </c>
@@ -4637,19 +4896,19 @@
         <v>40</v>
       </c>
       <c r="E45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F45" t="s">
         <v>100</v>
       </c>
       <c r="G45" t="s">
-        <v>156</v>
-      </c>
-      <c r="H45" s="1">
+        <v>155</v>
+      </c>
+      <c r="I45" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>71</v>
       </c>
@@ -4669,13 +4928,14 @@
         <v>100</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H46" t="s">
+        <v>185</v>
+      </c>
+      <c r="H46" s="3"/>
+      <c r="I46" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>73</v>
       </c>
@@ -4689,19 +4949,19 @@
         <v>41</v>
       </c>
       <c r="E47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F47" t="s">
         <v>100</v>
       </c>
       <c r="G47" t="s">
-        <v>157</v>
-      </c>
-      <c r="H47" s="1">
+        <v>156</v>
+      </c>
+      <c r="I47" s="1">
         <v>0.95</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>73</v>
       </c>
@@ -4715,19 +4975,19 @@
         <v>42</v>
       </c>
       <c r="E48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F48" t="s">
         <v>100</v>
       </c>
       <c r="G48" t="s">
-        <v>187</v>
-      </c>
-      <c r="H48" s="1">
+        <v>186</v>
+      </c>
+      <c r="I48" s="1">
         <v>0.03</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>73</v>
       </c>
@@ -4747,13 +5007,13 @@
         <v>100</v>
       </c>
       <c r="G49" t="s">
-        <v>155</v>
-      </c>
-      <c r="H49" t="s">
+        <v>154</v>
+      </c>
+      <c r="I49" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -4773,13 +5033,13 @@
         <v>100</v>
       </c>
       <c r="G50" t="s">
-        <v>170</v>
-      </c>
-      <c r="H50" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -4799,13 +5059,13 @@
         <v>100</v>
       </c>
       <c r="G51" t="s">
-        <v>170</v>
-      </c>
-      <c r="H51" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -4825,13 +5085,13 @@
         <v>100</v>
       </c>
       <c r="G52" t="s">
-        <v>191</v>
-      </c>
-      <c r="H52" s="1">
+        <v>190</v>
+      </c>
+      <c r="I52" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -4845,19 +5105,19 @@
         <v>54</v>
       </c>
       <c r="E53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F53" t="s">
         <v>100</v>
       </c>
       <c r="G53" t="s">
-        <v>174</v>
-      </c>
-      <c r="H53" s="1">
+        <v>173</v>
+      </c>
+      <c r="I53" s="1">
         <v>0.95</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>81</v>
       </c>
@@ -4871,19 +5131,22 @@
         <v>55</v>
       </c>
       <c r="E54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F54" t="s">
         <v>100</v>
       </c>
-      <c r="G54" t="s">
-        <v>151</v>
+      <c r="G54" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="H54" t="s">
+        <v>364</v>
+      </c>
+      <c r="I54" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>81</v>
       </c>
@@ -4897,19 +5160,22 @@
         <v>67</v>
       </c>
       <c r="E55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F55" t="s">
         <v>100</v>
       </c>
-      <c r="G55" t="s">
-        <v>188</v>
+      <c r="G55" s="9" t="s">
+        <v>187</v>
       </c>
       <c r="H55" t="s">
+        <v>365</v>
+      </c>
+      <c r="I55" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -4923,19 +5189,19 @@
         <v>56</v>
       </c>
       <c r="E56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F56" t="s">
         <v>100</v>
       </c>
       <c r="G56" t="s">
-        <v>168</v>
-      </c>
-      <c r="H56" s="1">
+        <v>167</v>
+      </c>
+      <c r="I56" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -4955,13 +5221,13 @@
         <v>100</v>
       </c>
       <c r="G57" t="s">
-        <v>183</v>
-      </c>
-      <c r="H57" t="s">
+        <v>182</v>
+      </c>
+      <c r="I57" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>84</v>
       </c>
@@ -4975,19 +5241,22 @@
         <v>57</v>
       </c>
       <c r="E58" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F58" t="s">
         <v>100</v>
       </c>
-      <c r="G58" t="s">
-        <v>154</v>
-      </c>
-      <c r="H58" s="1">
+      <c r="G58" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H58" t="s">
+        <v>366</v>
+      </c>
+      <c r="I58" s="1">
         <v>0.75</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -5001,19 +5270,22 @@
         <v>65</v>
       </c>
       <c r="E59" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F59" t="s">
         <v>100</v>
       </c>
-      <c r="G59" t="s">
-        <v>184</v>
+      <c r="G59" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="H59" t="s">
+        <v>367</v>
+      </c>
+      <c r="I59" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -5027,19 +5299,19 @@
         <v>58</v>
       </c>
       <c r="E60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F60" t="s">
         <v>100</v>
       </c>
       <c r="G60" t="s">
-        <v>169</v>
-      </c>
-      <c r="H60" s="1">
+        <v>168</v>
+      </c>
+      <c r="I60" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -5059,13 +5331,13 @@
         <v>100</v>
       </c>
       <c r="G61" t="s">
-        <v>185</v>
-      </c>
-      <c r="H61" t="s">
+        <v>184</v>
+      </c>
+      <c r="I61" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -5079,19 +5351,19 @@
         <v>59</v>
       </c>
       <c r="E62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F62" t="s">
         <v>100</v>
       </c>
       <c r="G62" t="s">
-        <v>156</v>
-      </c>
-      <c r="H62" s="1">
+        <v>155</v>
+      </c>
+      <c r="I62" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -5111,13 +5383,13 @@
         <v>100</v>
       </c>
       <c r="G63" t="s">
-        <v>186</v>
-      </c>
-      <c r="H63" t="s">
+        <v>185</v>
+      </c>
+      <c r="I63" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -5131,19 +5403,19 @@
         <v>60</v>
       </c>
       <c r="E64" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F64" t="s">
         <v>100</v>
       </c>
       <c r="G64" t="s">
-        <v>157</v>
-      </c>
-      <c r="H64" s="1">
+        <v>156</v>
+      </c>
+      <c r="I64" s="1">
         <v>0.95</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>90</v>
       </c>
@@ -5157,19 +5429,19 @@
         <v>61</v>
       </c>
       <c r="E65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F65" t="s">
         <v>100</v>
       </c>
       <c r="G65" t="s">
-        <v>187</v>
-      </c>
-      <c r="H65" s="1">
+        <v>186</v>
+      </c>
+      <c r="I65" s="1">
         <v>0.03</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>90</v>
       </c>
@@ -5189,13 +5461,13 @@
         <v>100</v>
       </c>
       <c r="G66" t="s">
-        <v>155</v>
-      </c>
-      <c r="H66" t="s">
+        <v>154</v>
+      </c>
+      <c r="I66" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>83</v>
       </c>
@@ -5215,14 +5487,14 @@
         <v>100</v>
       </c>
       <c r="G67" t="s">
-        <v>170</v>
-      </c>
-      <c r="H67" s="1">
+        <v>169</v>
+      </c>
+      <c r="I67" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I67">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J67">
     <sortCondition ref="B2:B67"/>
     <sortCondition ref="D2:D67"/>
   </sortState>
@@ -5281,10 +5553,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5304,7 +5576,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5321,10 +5593,10 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -5341,10 +5613,10 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -5361,10 +5633,10 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -5381,10 +5653,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -5404,7 +5676,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -5421,10 +5693,10 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -5441,10 +5713,10 @@
         <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -5461,10 +5733,10 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -5484,7 +5756,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -5501,10 +5773,10 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -5524,7 +5796,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -5541,10 +5813,10 @@
         <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -5561,10 +5833,10 @@
         <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -5584,7 +5856,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -5604,7 +5876,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -5624,7 +5896,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -5644,7 +5916,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -5664,7 +5936,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -5684,7 +5956,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -5704,7 +5976,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -5721,10 +5993,10 @@
         <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -5738,13 +6010,13 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -5761,10 +6033,10 @@
         <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -5778,13 +6050,13 @@
         <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -5801,10 +6073,10 @@
         <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -5818,13 +6090,13 @@
         <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -5841,10 +6113,10 @@
         <v>16</v>
       </c>
       <c r="E30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -5858,13 +6130,13 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -5881,10 +6153,10 @@
         <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -5898,13 +6170,13 @@
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -5918,13 +6190,13 @@
         <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -5938,13 +6210,13 @@
         <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -5958,13 +6230,13 @@
         <v>28</v>
       </c>
       <c r="D36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -5981,10 +6253,10 @@
         <v>19</v>
       </c>
       <c r="E37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -5998,13 +6270,13 @@
         <v>51</v>
       </c>
       <c r="D38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -6018,13 +6290,13 @@
         <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -6041,10 +6313,10 @@
         <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -6061,10 +6333,10 @@
         <v>21</v>
       </c>
       <c r="E41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F41" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -6081,10 +6353,10 @@
         <v>26</v>
       </c>
       <c r="E42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F42" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -6101,10 +6373,10 @@
         <v>22</v>
       </c>
       <c r="E43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F43" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -6118,13 +6390,13 @@
         <v>48</v>
       </c>
       <c r="D44" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -6141,10 +6413,10 @@
         <v>23</v>
       </c>
       <c r="E45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -6158,13 +6430,13 @@
         <v>47</v>
       </c>
       <c r="D46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -6181,10 +6453,10 @@
         <v>24</v>
       </c>
       <c r="E47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -6198,13 +6470,13 @@
         <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -6221,10 +6493,10 @@
         <v>25</v>
       </c>
       <c r="E49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -6238,13 +6510,13 @@
         <v>45</v>
       </c>
       <c r="D50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -6258,13 +6530,13 @@
         <v>42</v>
       </c>
       <c r="D51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -6278,13 +6550,13 @@
         <v>43</v>
       </c>
       <c r="D52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -6298,13 +6570,13 @@
         <v>44</v>
       </c>
       <c r="D53" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -6318,13 +6590,13 @@
         <v>50</v>
       </c>
       <c r="D54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -6338,13 +6610,13 @@
         <v>53</v>
       </c>
       <c r="D55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -6361,10 +6633,10 @@
         <v>29</v>
       </c>
       <c r="E56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -6378,13 +6650,13 @@
         <v>72</v>
       </c>
       <c r="D57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -6398,13 +6670,13 @@
         <v>56</v>
       </c>
       <c r="D58" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -6421,10 +6693,10 @@
         <v>30</v>
       </c>
       <c r="E59" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F59" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -6441,10 +6713,10 @@
         <v>31</v>
       </c>
       <c r="E60" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F60" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -6461,10 +6733,10 @@
         <v>36</v>
       </c>
       <c r="E61" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F61" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -6481,10 +6753,10 @@
         <v>32</v>
       </c>
       <c r="E62" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F62" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -6498,13 +6770,13 @@
         <v>69</v>
       </c>
       <c r="D63" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -6521,10 +6793,10 @@
         <v>33</v>
       </c>
       <c r="E64" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -6538,13 +6810,13 @@
         <v>68</v>
       </c>
       <c r="D65" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -6561,10 +6833,10 @@
         <v>34</v>
       </c>
       <c r="E66" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F66" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -6578,13 +6850,13 @@
         <v>67</v>
       </c>
       <c r="D67" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -6601,10 +6873,10 @@
         <v>35</v>
       </c>
       <c r="E68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F68" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -6618,13 +6890,13 @@
         <v>66</v>
       </c>
       <c r="D69" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -6638,13 +6910,13 @@
         <v>63</v>
       </c>
       <c r="D70" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E70" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F70" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -6658,13 +6930,13 @@
         <v>64</v>
       </c>
       <c r="D71" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F71" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -6678,13 +6950,13 @@
         <v>65</v>
       </c>
       <c r="D72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -6698,13 +6970,13 @@
         <v>71</v>
       </c>
       <c r="D73" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated transitions to correct specificity problem
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D6EE5D-55AE-3F4E-BB1D-D1DAA6A42188}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10517918-CCD5-2448-A577-AB86BAD1AD18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" activeTab="2" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="381">
   <si>
     <t>NumberFrom</t>
   </si>
@@ -1137,39 +1137,6 @@
     <t>NewModel</t>
   </si>
   <si>
-    <t>b*(sens2 + (1-spec2))</t>
-  </si>
-  <si>
-    <t>1 - b*(sens2 + (1-spec2))</t>
-  </si>
-  <si>
-    <t>d*sens2/(sens2 + (1-spec2))</t>
-  </si>
-  <si>
-    <t>1 - d*sens2/(sens2 + (1-spec2))</t>
-  </si>
-  <si>
-    <t>v*w*z1*b*(sens*x + (1-spec*x))</t>
-  </si>
-  <si>
-    <t>(1-v)*w*z1*b*(sens*x + (1-spec*x))</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> w*z2*(1-b*(sens*x + (1-spec*x)))</t>
-  </si>
-  <si>
-    <t>d*sens*x/(sens*x + (1 - spec*x))</t>
-  </si>
-  <si>
-    <t>1 - d*sens*x/(sens*x + (1 - spec*x))</t>
-  </si>
-  <si>
-    <t>[sens*sens2*x + (1-spec*x)*(1-spec2)] / [sens*x + (1-spec*x)]</t>
-  </si>
-  <si>
-    <t>1 - [sens*sens2*x + (1-spec*x)*(1-spec2)] / [sens*x + (1-spec*x)]</t>
-  </si>
-  <si>
     <t>Interreaderagreement</t>
   </si>
   <si>
@@ -1177,6 +1144,48 @@
   </si>
   <si>
     <t>1-p  this was likely causing strange results before</t>
+  </si>
+  <si>
+    <t>b*(sens2) + (1-b)*(1-spec2))</t>
+  </si>
+  <si>
+    <t>1 - b*(sens2) + (1-b)*(1-spec2))</t>
+  </si>
+  <si>
+    <t>1 - (b*(sens2) + (1-b)*(1-spec2)))</t>
+  </si>
+  <si>
+    <t>v*w*z1*(b*sens*x + (1-b)*(1-spec*x))</t>
+  </si>
+  <si>
+    <t>(1-v)*w*z1*(b*sens*x + (1-b)*(1-spec*x))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> w*z2*(1-(b*sens*x + (1-b)*(1-spec*x)))</t>
+  </si>
+  <si>
+    <t>d* (b*sens2) / (b*sens2 + (1-b)*(1-spec2))</t>
+  </si>
+  <si>
+    <t>1 - (d* (b*sens2) / (b*sens2 + (1-b)*(1-spec2)))</t>
+  </si>
+  <si>
+    <t>d* (b*sens*x) / (b*sens*x + (1-b)*(1-spec*x))</t>
+  </si>
+  <si>
+    <t>1 - d* (b*sens*x) / (b*sens*x + (1-b)*(1-spec*x))</t>
+  </si>
+  <si>
+    <t>((b*sens*x)*sens2 + (1-b)*(1-spec*x)*(1-spec2))) / ((b*sens*x + (1-b)*(1-spec*x))</t>
+  </si>
+  <si>
+    <t>1 - ((b*sens*x)*sens2 + (1-b)*(1-spec*x)*(1-spec2))) / ((b*sens*x + (1-b)*(1-spec*x))</t>
+  </si>
+  <si>
+    <t>d* (b*sens*x)*sens2 / ((b*sens*x)*sens2 + (1-b)*(1-spec*x)*(1-spec2)))</t>
+  </si>
+  <si>
+    <t>1 - d* (b*sens*x)*sens2 / ((b*sens*x)*sens2 + (1-b)*(1-spec*x)*(1-spec2)))</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1259,6 +1268,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1576,8 +1587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707EB61A-F669-6B48-8A71-B654C41C6040}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2964,7 +2975,7 @@
         <v>172</v>
       </c>
       <c r="B25" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="C25" t="s">
         <v>126</v>
@@ -3077,7 +3088,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="102" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>174</v>
       </c>
@@ -3224,7 +3235,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1">
-        <f t="shared" ref="O29:P30" si="0">4633/4781</f>
+        <f t="shared" ref="O29:O30" si="0">4633/4781</f>
         <v>0.96904413302656345</v>
       </c>
       <c r="P29" s="1">
@@ -3615,8 +3626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D1F24D-5226-E34A-88F5-702AF231CD7B}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3624,8 +3635,9 @@
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="34.5" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="30.83203125" customWidth="1"/>
+    <col min="8" max="8" width="60.6640625" customWidth="1"/>
     <col min="9" max="9" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="32.5" customWidth="1"/>
   </cols>
@@ -3769,7 +3781,7 @@
         <v>150</v>
       </c>
       <c r="H5" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="I5" t="s">
         <v>105</v>
@@ -3798,7 +3810,7 @@
         <v>187</v>
       </c>
       <c r="H6" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="I6" t="s">
         <v>109</v>
@@ -3882,7 +3894,7 @@
         <v>153</v>
       </c>
       <c r="H9" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="I9" s="1">
         <v>0.75</v>
@@ -3914,7 +3926,7 @@
         <v>183</v>
       </c>
       <c r="H10" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="I10" t="s">
         <v>109</v>
@@ -4192,7 +4204,7 @@
         <v>252</v>
       </c>
       <c r="H20" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>260</v>
@@ -4224,7 +4236,7 @@
         <v>251</v>
       </c>
       <c r="H21" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>261</v>
@@ -4253,7 +4265,7 @@
         <v>250</v>
       </c>
       <c r="H22" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>262</v>
@@ -4311,10 +4323,10 @@
         <v>100</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="H24" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="I24" s="1">
         <v>0.1</v>
@@ -4375,7 +4387,7 @@
         <v>153</v>
       </c>
       <c r="H26" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="I26" s="1">
         <v>0.75</v>
@@ -4407,7 +4419,7 @@
         <v>183</v>
       </c>
       <c r="H27" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="I27" t="s">
         <v>109</v>
@@ -4679,7 +4691,7 @@
         <v>172</v>
       </c>
       <c r="H37" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="I37" s="1">
         <v>0.98</v>
@@ -4708,7 +4720,7 @@
         <v>181</v>
       </c>
       <c r="H38" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="I38" s="1">
         <v>0.02</v>
@@ -4765,6 +4777,7 @@
       <c r="G40" t="s">
         <v>182</v>
       </c>
+      <c r="H40" s="10"/>
       <c r="I40" t="s">
         <v>109</v>
       </c>
@@ -4791,8 +4804,8 @@
       <c r="G41" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="H41" t="s">
-        <v>366</v>
+      <c r="H41" s="11" t="s">
+        <v>379</v>
       </c>
       <c r="I41" s="1">
         <v>0.75</v>
@@ -4823,8 +4836,8 @@
       <c r="G42" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="H42" t="s">
-        <v>367</v>
+      <c r="H42" s="11" t="s">
+        <v>380</v>
       </c>
       <c r="I42" t="s">
         <v>109</v>
@@ -5140,7 +5153,7 @@
         <v>150</v>
       </c>
       <c r="H54" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="I54" t="s">
         <v>105</v>
@@ -5169,7 +5182,7 @@
         <v>187</v>
       </c>
       <c r="H55" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="I55" t="s">
         <v>120</v>
@@ -5250,7 +5263,7 @@
         <v>153</v>
       </c>
       <c r="H58" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="I58" s="1">
         <v>0.75</v>
@@ -5279,7 +5292,7 @@
         <v>183</v>
       </c>
       <c r="H59" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="I59" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
update parameter inputs for new scenarios
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10517918-CCD5-2448-A577-AB86BAD1AD18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544C43BE-5D14-A34E-A0C6-1D6151EC1886}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="2" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="382">
   <si>
     <t>NumberFrom</t>
   </si>
@@ -1104,15 +1104,9 @@
     <t>sens</t>
   </si>
   <si>
-    <t>OraQuick sensitivity</t>
-  </si>
-  <si>
     <t>spec</t>
   </si>
   <si>
-    <t>OraQuick specificity</t>
-  </si>
-  <si>
     <t>f1</t>
   </si>
   <si>
@@ -1128,12 +1122,6 @@
     <t>spec2</t>
   </si>
   <si>
-    <t>Retest sensitivity</t>
-  </si>
-  <si>
-    <t>Retest specificity</t>
-  </si>
-  <si>
     <t>NewModel</t>
   </si>
   <si>
@@ -1186,6 +1174,21 @@
   </si>
   <si>
     <t>1 - d* (b*sens*x)*sens2 / ((b*sens*x)*sens2 + (1-b)*(1-spec*x)*(1-spec2)))</t>
+  </si>
+  <si>
+    <t>Facility based</t>
+  </si>
+  <si>
+    <t>Self-test sensitivity</t>
+  </si>
+  <si>
+    <t>Self-test specificity</t>
+  </si>
+  <si>
+    <t>Facility-based sensitivity</t>
+  </si>
+  <si>
+    <t>Facility-based specificity</t>
   </si>
 </sst>
 </file>
@@ -1587,8 +1590,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707EB61A-F669-6B48-8A71-B654C41C6040}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="T8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="U36" sqref="U36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1957,7 +1963,7 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>5.63</v>
       </c>
       <c r="I6" t="s">
         <v>241</v>
@@ -1966,7 +1972,7 @@
         <v>5</v>
       </c>
       <c r="K6">
-        <v>5</v>
+        <v>5.63</v>
       </c>
       <c r="N6" t="s">
         <v>267</v>
@@ -1975,13 +1981,13 @@
         <v>5</v>
       </c>
       <c r="P6">
-        <v>5</v>
+        <v>5.63</v>
       </c>
       <c r="T6">
         <v>5</v>
       </c>
       <c r="U6">
-        <v>5</v>
+        <v>5.63</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
@@ -2001,15 +2007,13 @@
         <v>31.24</v>
       </c>
       <c r="F7">
-        <f>E7*Sheet1!F3/Sheet1!E3</f>
-        <v>32.756045402980575</v>
+        <v>32.76</v>
       </c>
       <c r="I7" t="s">
         <v>319</v>
       </c>
       <c r="K7">
-        <f>K34*2</f>
-        <v>42.860012210275542</v>
+        <v>42.87</v>
       </c>
       <c r="N7" t="s">
         <v>326</v>
@@ -2018,8 +2022,7 @@
         <v>1</v>
       </c>
       <c r="P7">
-        <f>35/6.91</f>
-        <v>5.0651230101302458</v>
+        <v>5.07</v>
       </c>
       <c r="S7" t="s">
         <v>336</v>
@@ -2120,7 +2123,7 @@
         <v>784.36797351282996</v>
       </c>
       <c r="I9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J9">
         <v>1552</v>
@@ -2428,7 +2431,7 @@
         <v>0.1</v>
       </c>
       <c r="F15" s="1">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -2439,7 +2442,7 @@
         <v>0.1</v>
       </c>
       <c r="K15" s="1">
-        <v>0.1</v>
+        <v>0.36</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -2450,7 +2453,7 @@
         <v>0.1</v>
       </c>
       <c r="P15" s="1">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2459,7 +2462,7 @@
         <v>0.1</v>
       </c>
       <c r="U15" s="1">
-        <v>0.1</v>
+        <v>0.36</v>
       </c>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
@@ -2485,7 +2488,7 @@
         <v>0.05</v>
       </c>
       <c r="F16" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -2496,7 +2499,7 @@
         <v>0.05</v>
       </c>
       <c r="K16" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -2507,7 +2510,7 @@
         <v>0.05</v>
       </c>
       <c r="P16" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -2516,7 +2519,7 @@
         <v>0.05</v>
       </c>
       <c r="U16" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
@@ -2926,7 +2929,7 @@
         <v>0.92</v>
       </c>
       <c r="F24" s="1">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -2937,7 +2940,7 @@
         <v>0.9</v>
       </c>
       <c r="K24" s="1">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -2948,7 +2951,7 @@
         <v>0.96</v>
       </c>
       <c r="P24" s="1">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -2959,7 +2962,7 @@
         <v>0.46</v>
       </c>
       <c r="U24" s="1">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
@@ -2975,7 +2978,7 @@
         <v>172</v>
       </c>
       <c r="B25" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C25" t="s">
         <v>126</v>
@@ -3174,7 +3177,7 @@
         <v>0.8</v>
       </c>
       <c r="K28" s="1">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -3197,7 +3200,7 @@
         <v>0.9</v>
       </c>
       <c r="U28" s="1">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
@@ -3282,7 +3285,7 @@
         <v>0.8</v>
       </c>
       <c r="K30" s="1">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -3303,7 +3306,7 @@
         <v>0.5</v>
       </c>
       <c r="U30" s="1">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
@@ -3365,10 +3368,7 @@
         <v>352</v>
       </c>
       <c r="B32" t="s">
-        <v>353</v>
-      </c>
-      <c r="C32" t="s">
-        <v>126</v>
+        <v>378</v>
       </c>
       <c r="F32" s="8">
         <v>0.98</v>
@@ -3391,10 +3391,10 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B33" t="s">
-        <v>355</v>
+        <v>379</v>
       </c>
       <c r="C33" t="s">
         <v>126</v>
@@ -3420,10 +3420,10 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B34" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E34">
         <v>2.66</v>
@@ -3460,30 +3460,33 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B35" t="s">
-        <v>361</v>
+        <v>380</v>
+      </c>
+      <c r="C35" t="s">
+        <v>377</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="K35">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="P35">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="U35" s="8">
-        <v>1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B36" t="s">
-        <v>362</v>
+        <v>381</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -3626,7 +3629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D1F24D-5226-E34A-88F5-702AF231CD7B}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
+    <sheetView topLeftCell="F28" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
@@ -3665,7 +3668,7 @@
         <v>97</v>
       </c>
       <c r="H1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="I1" t="s">
         <v>103</v>
@@ -3781,7 +3784,7 @@
         <v>150</v>
       </c>
       <c r="H5" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="I5" t="s">
         <v>105</v>
@@ -3810,7 +3813,7 @@
         <v>187</v>
       </c>
       <c r="H6" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="I6" t="s">
         <v>109</v>
@@ -3894,7 +3897,7 @@
         <v>153</v>
       </c>
       <c r="H9" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="I9" s="1">
         <v>0.75</v>
@@ -3926,7 +3929,7 @@
         <v>183</v>
       </c>
       <c r="H10" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="I10" t="s">
         <v>109</v>
@@ -4204,7 +4207,7 @@
         <v>252</v>
       </c>
       <c r="H20" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>260</v>
@@ -4236,7 +4239,7 @@
         <v>251</v>
       </c>
       <c r="H21" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>261</v>
@@ -4265,7 +4268,7 @@
         <v>250</v>
       </c>
       <c r="H22" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>262</v>
@@ -4323,10 +4326,10 @@
         <v>100</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="H24" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="I24" s="1">
         <v>0.1</v>
@@ -4387,7 +4390,7 @@
         <v>153</v>
       </c>
       <c r="H26" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="I26" s="1">
         <v>0.75</v>
@@ -4419,7 +4422,7 @@
         <v>183</v>
       </c>
       <c r="H27" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="I27" t="s">
         <v>109</v>
@@ -4691,7 +4694,7 @@
         <v>172</v>
       </c>
       <c r="H37" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="I37" s="1">
         <v>0.98</v>
@@ -4720,7 +4723,7 @@
         <v>181</v>
       </c>
       <c r="H38" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="I38" s="1">
         <v>0.02</v>
@@ -4805,7 +4808,7 @@
         <v>153</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="I41" s="1">
         <v>0.75</v>
@@ -4837,7 +4840,7 @@
         <v>183</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="I42" t="s">
         <v>109</v>
@@ -5153,7 +5156,7 @@
         <v>150</v>
       </c>
       <c r="H54" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="I54" t="s">
         <v>105</v>
@@ -5182,7 +5185,7 @@
         <v>187</v>
       </c>
       <c r="H55" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I55" t="s">
         <v>120</v>
@@ -5263,7 +5266,7 @@
         <v>153</v>
       </c>
       <c r="H58" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="I58" s="1">
         <v>0.75</v>
@@ -5292,7 +5295,7 @@
         <v>183</v>
       </c>
       <c r="H59" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="I59" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
update scenarios in code
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544C43BE-5D14-A34E-A0C6-1D6151EC1886}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB39E94-FB8B-0A42-9547-02E23C8FD36B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="390">
   <si>
     <t>NumberFrom</t>
   </si>
@@ -1189,6 +1189,30 @@
   </si>
   <si>
     <t>Facility-based specificity</t>
+  </si>
+  <si>
+    <t>highup</t>
+  </si>
+  <si>
+    <t>lowup</t>
+  </si>
+  <si>
+    <t>HighUptakePercent</t>
+  </si>
+  <si>
+    <t>LowUptakePercent</t>
+  </si>
+  <si>
+    <t>WithHighSub</t>
+  </si>
+  <si>
+    <t>WithLowSub</t>
+  </si>
+  <si>
+    <t>highsub</t>
+  </si>
+  <si>
+    <t>lowsub</t>
   </si>
 </sst>
 </file>
@@ -1588,13 +1612,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707EB61A-F669-6B48-8A71-B654C41C6040}">
-  <dimension ref="A1:Y36"/>
+  <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="T8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="T12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U36" sqref="U36"/>
+      <selection pane="bottomRight" activeCell="U41" sqref="U41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3499,6 +3523,86 @@
       </c>
       <c r="U36">
         <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>382</v>
+      </c>
+      <c r="B37" t="s">
+        <v>384</v>
+      </c>
+      <c r="F37">
+        <v>0.12</v>
+      </c>
+      <c r="K37">
+        <v>0.45</v>
+      </c>
+      <c r="P37">
+        <v>0.09</v>
+      </c>
+      <c r="U37">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>383</v>
+      </c>
+      <c r="B38" t="s">
+        <v>385</v>
+      </c>
+      <c r="F38">
+        <v>0.05</v>
+      </c>
+      <c r="K38">
+        <v>0.2</v>
+      </c>
+      <c r="P38">
+        <v>0.04</v>
+      </c>
+      <c r="U38">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>388</v>
+      </c>
+      <c r="B39" t="s">
+        <v>386</v>
+      </c>
+      <c r="F39">
+        <v>0.11</v>
+      </c>
+      <c r="K39">
+        <v>0.41</v>
+      </c>
+      <c r="P39">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="U39">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>389</v>
+      </c>
+      <c r="B40" t="s">
+        <v>387</v>
+      </c>
+      <c r="F40">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="K40">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="P40">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="U40">
+        <v>0.33500000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a few more final updates before sending updated paper
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/HCVST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB39E94-FB8B-0A42-9547-02E23C8FD36B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F89DA5-23E5-A644-91E1-554559DAD9C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" xr2:uid="{9426A51E-D1CB-CD4D-946E-02589EA87648}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="389">
   <si>
     <t>NumberFrom</t>
   </si>
@@ -1203,22 +1203,22 @@
     <t>LowUptakePercent</t>
   </si>
   <si>
-    <t>WithHighSub</t>
-  </si>
-  <si>
-    <t>WithLowSub</t>
-  </si>
-  <si>
     <t>highsub</t>
   </si>
   <si>
     <t>lowsub</t>
+  </si>
+  <si>
+    <t>DON'T USE?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1282,7 +1282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1297,6 +1297,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1615,10 +1616,10 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="T12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U41" sqref="U41"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2396,7 +2397,7 @@
         <f>29465/F2</f>
         <v>0.12581127241673784</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
         <v>242</v>
@@ -2455,7 +2456,7 @@
         <v>0.1</v>
       </c>
       <c r="F15" s="1">
-        <v>0.09</v>
+        <v>7.8E-2</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -2466,7 +2467,7 @@
         <v>0.1</v>
       </c>
       <c r="K15" s="1">
-        <v>0.36</v>
+        <v>0.31</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -2477,7 +2478,7 @@
         <v>0.1</v>
       </c>
       <c r="P15" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2486,7 +2487,7 @@
         <v>0.1</v>
       </c>
       <c r="U15" s="1">
-        <v>0.36</v>
+        <v>0.31</v>
       </c>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
@@ -3533,16 +3534,16 @@
         <v>384</v>
       </c>
       <c r="F37">
-        <v>0.12</v>
+        <v>0.1008</v>
       </c>
       <c r="K37">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="P37">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="U37">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
@@ -3553,56 +3554,56 @@
         <v>385</v>
       </c>
       <c r="F38">
-        <v>0.05</v>
+        <v>3.78E-2</v>
       </c>
       <c r="K38">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="P38">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="U38">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>386</v>
+      </c>
+      <c r="B39" t="s">
         <v>388</v>
       </c>
-      <c r="B39" t="s">
-        <v>386</v>
-      </c>
       <c r="F39">
-        <v>0.11</v>
+        <v>5.2920000000000002E-2</v>
       </c>
       <c r="K39">
-        <v>0.41</v>
+        <v>0.21</v>
       </c>
       <c r="P39">
-        <v>8.2000000000000003E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="U39">
-        <v>0.41</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B40" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F40">
-        <v>8.6999999999999994E-2</v>
+        <v>7.1819999999999995E-2</v>
       </c>
       <c r="K40">
-        <v>0.33500000000000002</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="P40">
-        <v>6.7000000000000004E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="U40">
-        <v>0.33500000000000002</v>
+        <v>0.28499999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>